<commit_message>
Modify path according to new file system.
</commit_message>
<xml_diff>
--- a/Results/report.xlsx
+++ b/Results/report.xlsx
@@ -414,19 +414,19 @@
         <v>38749</v>
       </c>
       <c r="B2" t="n">
-        <v>0.04019497</v>
+        <v>0.03108962</v>
       </c>
       <c r="C2" t="n">
-        <v>1.604637702929827</v>
+        <v>1.443966035204057</v>
       </c>
       <c r="D2" t="n">
-        <v>1.04019497</v>
+        <v>1.03108962</v>
       </c>
       <c r="E2" t="n">
         <v>0.042997</v>
       </c>
       <c r="F2" t="n">
-        <v>-0.002802030000000004</v>
+        <v>-0.01190738</v>
       </c>
       <c r="G2" t="n">
         <v>1.042997</v>
@@ -437,19 +437,19 @@
         <v>38777</v>
       </c>
       <c r="B3" t="n">
-        <v>0.01228691836734694</v>
+        <v>0.01615942857142857</v>
       </c>
       <c r="C3" t="n">
-        <v>1.157826525041433</v>
+        <v>1.21211050201982</v>
       </c>
       <c r="D3" t="n">
-        <v>1.052975760682515</v>
+        <v>1.047751439065131</v>
       </c>
       <c r="E3" t="n">
         <v>0.007673</v>
       </c>
       <c r="F3" t="n">
-        <v>0.004613918367346937</v>
+        <v>0.008486428571428572</v>
       </c>
       <c r="G3" t="n">
         <v>1.050999915981</v>
@@ -460,19 +460,19 @@
         <v>38808</v>
       </c>
       <c r="B4" t="n">
-        <v>0.09516287096774194</v>
+        <v>0.099395306122449</v>
       </c>
       <c r="C4" t="n">
-        <v>2.976764920879751</v>
+        <v>3.117787711042751</v>
       </c>
       <c r="D4" t="n">
-        <v>1.153179957128505</v>
+        <v>1.151893014091247</v>
       </c>
       <c r="E4" t="n">
         <v>0.104854</v>
       </c>
       <c r="F4" t="n">
-        <v>-0.009691129032258064</v>
+        <v>-0.005458693877551005</v>
       </c>
       <c r="G4" t="n">
         <v>1.161201461171272</v>
@@ -483,19 +483,19 @@
         <v>38838</v>
       </c>
       <c r="B5" t="n">
-        <v>0.2592448631578947</v>
+        <v>0.2848055520833333</v>
       </c>
       <c r="C5" t="n">
-        <v>15.89725918682262</v>
+        <v>20.23246771592801</v>
       </c>
       <c r="D5" t="n">
-        <v>1.452135937310711</v>
+        <v>1.479958539910439</v>
       </c>
       <c r="E5" t="n">
         <v>0.164712</v>
       </c>
       <c r="F5" t="n">
-        <v>0.09453286315789475</v>
+        <v>0.1200935520833333</v>
       </c>
       <c r="G5" t="n">
         <v>1.352465276243714</v>
@@ -506,19 +506,19 @@
         <v>38869</v>
       </c>
       <c r="B6" t="n">
-        <v>0.09767205263157895</v>
+        <v>0.07047415624999999</v>
       </c>
       <c r="C6" t="n">
-        <v>3.059646717337283</v>
+        <v>2.264197165988822</v>
       </c>
       <c r="D6" t="n">
-        <v>1.59396903500793</v>
+        <v>1.584257369295609</v>
       </c>
       <c r="E6" t="n">
         <v>0.02088</v>
       </c>
       <c r="F6" t="n">
-        <v>0.07679205263157896</v>
+        <v>0.04959415624999999</v>
       </c>
       <c r="G6" t="n">
         <v>1.380704751211683</v>
@@ -529,19 +529,19 @@
         <v>38899</v>
       </c>
       <c r="B7" t="n">
-        <v>-0.01186583157894737</v>
+        <v>-0.02926641052631579</v>
       </c>
       <c r="C7" t="n">
-        <v>0.8665447648433855</v>
+        <v>0.7001654700211591</v>
       </c>
       <c r="D7" t="n">
-        <v>1.575055266896469</v>
+        <v>1.537891842746463</v>
       </c>
       <c r="E7" t="n">
         <v>-0.07147300000000001</v>
       </c>
       <c r="F7" t="n">
-        <v>0.05960716842105264</v>
+        <v>0.04220658947368422</v>
       </c>
       <c r="G7" t="n">
         <v>1.28202164052833</v>
@@ -552,19 +552,19 @@
         <v>38930</v>
       </c>
       <c r="B8" t="n">
-        <v>0.02468251086956521</v>
+        <v>0.03100192391304348</v>
       </c>
       <c r="C8" t="n">
-        <v>1.339898452526568</v>
+        <v>1.442492980490683</v>
       </c>
       <c r="D8" t="n">
-        <v>1.613931585641807</v>
+        <v>1.585569448641779</v>
       </c>
       <c r="E8" t="n">
         <v>0.034273</v>
       </c>
       <c r="F8" t="n">
-        <v>-0.009590489130434792</v>
+        <v>-0.003271076086956523</v>
       </c>
       <c r="G8" t="n">
         <v>1.325960368214158</v>
@@ -575,19 +575,19 @@
         <v>38961</v>
       </c>
       <c r="B9" t="n">
-        <v>0.04384070212765957</v>
+        <v>0.06491767368421053</v>
       </c>
       <c r="C9" t="n">
-        <v>1.673442235330533</v>
+        <v>2.127122087781593</v>
       </c>
       <c r="D9" t="n">
-        <v>1.684687479542351</v>
+        <v>1.688500928712359</v>
       </c>
       <c r="E9" t="n">
         <v>0.048241</v>
       </c>
       <c r="F9" t="n">
-        <v>-0.004400297872340427</v>
+        <v>0.01667667368421053</v>
       </c>
       <c r="G9" t="n">
         <v>1.389926022337177</v>
@@ -598,19 +598,19 @@
         <v>38991</v>
       </c>
       <c r="B10" t="n">
-        <v>-0.003483610526315784</v>
+        <v>-0.004599374999999998</v>
       </c>
       <c r="C10" t="n">
-        <v>0.9589883913599703</v>
+        <v>0.9461824952253329</v>
       </c>
       <c r="D10" t="n">
-        <v>1.678818684505065</v>
+        <v>1.680734879753363</v>
       </c>
       <c r="E10" t="n">
         <v>0.043612</v>
       </c>
       <c r="F10" t="n">
-        <v>-0.04709561052631578</v>
+        <v>-0.04821137499999999</v>
       </c>
       <c r="G10" t="n">
         <v>1.450543476023346</v>
@@ -621,19 +621,19 @@
         <v>39022</v>
       </c>
       <c r="B11" t="n">
-        <v>0.03581967368421052</v>
+        <v>0.03438626595744681</v>
       </c>
       <c r="C11" t="n">
-        <v>1.525491758151065</v>
+        <v>1.500351258471692</v>
       </c>
       <c r="D11" t="n">
-        <v>1.738953421958991</v>
+        <v>1.738529076332519</v>
       </c>
       <c r="E11" t="n">
         <v>0.170635</v>
       </c>
       <c r="F11" t="n">
-        <v>-0.1348153263157895</v>
+        <v>-0.1362487340425532</v>
       </c>
       <c r="G11" t="n">
         <v>1.698056962054589</v>
@@ -644,19 +644,19 @@
         <v>39052</v>
       </c>
       <c r="B12" t="n">
-        <v>0.08601872340425533</v>
+        <v>0.06514616842105264</v>
       </c>
       <c r="C12" t="n">
-        <v>2.691830767408989</v>
+        <v>2.132605443358822</v>
       </c>
       <c r="D12" t="n">
-        <v>1.888535975375365</v>
+        <v>1.851787584344174</v>
       </c>
       <c r="E12" t="n">
         <v>0.190561</v>
       </c>
       <c r="F12" t="n">
-        <v>-0.1045422765957447</v>
+        <v>-0.1254148315789473</v>
       </c>
       <c r="G12" t="n">
         <v>2.021640394800674</v>
@@ -667,19 +667,19 @@
         <v>39083</v>
       </c>
       <c r="B13" t="n">
-        <v>0.2326945978260869</v>
+        <v>0.2606744842105264</v>
       </c>
       <c r="C13" t="n">
-        <v>12.31022278710726</v>
+        <v>16.11519461794067</v>
       </c>
       <c r="D13" t="n">
-        <v>2.327988094645432</v>
+        <v>2.334501357760549</v>
       </c>
       <c r="E13" t="n">
         <v>0.168683</v>
       </c>
       <c r="F13" t="n">
-        <v>0.06401159782608692</v>
+        <v>0.09199148421052636</v>
       </c>
       <c r="G13" t="n">
         <v>2.362656761516836</v>
@@ -690,19 +690,19 @@
         <v>39114</v>
       </c>
       <c r="B14" t="n">
-        <v>0.2040252934782608</v>
+        <v>0.1942958404255319</v>
       </c>
       <c r="C14" t="n">
-        <v>9.281695681998377</v>
+        <v>8.420599977633991</v>
       </c>
       <c r="D14" t="n">
-        <v>2.802956548869364</v>
+        <v>2.78808526104118</v>
       </c>
       <c r="E14" t="n">
         <v>0.06675399999999999</v>
       </c>
       <c r="F14" t="n">
-        <v>0.1372712934782608</v>
+        <v>0.127541840425532</v>
       </c>
       <c r="G14" t="n">
         <v>2.520373550975131</v>
@@ -713,19 +713,19 @@
         <v>39142</v>
       </c>
       <c r="B15" t="n">
-        <v>0.2200433333333333</v>
+        <v>0.1792582916666667</v>
       </c>
       <c r="C15" t="n">
-        <v>10.87684836228738</v>
+        <v>7.232813432129632</v>
       </c>
       <c r="D15" t="n">
-        <v>3.419728451071075</v>
+        <v>3.287872661956434</v>
       </c>
       <c r="E15" t="n">
         <v>0.093222</v>
       </c>
       <c r="F15" t="n">
-        <v>0.1268213333333333</v>
+        <v>0.08603629166666665</v>
       </c>
       <c r="G15" t="n">
         <v>2.755327814144135</v>
@@ -736,19 +736,19 @@
         <v>39173</v>
       </c>
       <c r="B16" t="n">
-        <v>0.370318935483871</v>
+        <v>0.3577411052631579</v>
       </c>
       <c r="C16" t="n">
-        <v>43.83892618725983</v>
+        <v>39.24674072417004</v>
       </c>
       <c r="D16" t="n">
-        <v>4.686118650715623</v>
+        <v>4.46407986200925</v>
       </c>
       <c r="E16" t="n">
         <v>0.279292</v>
       </c>
       <c r="F16" t="n">
-        <v>0.09102693548387097</v>
+        <v>0.0784491052631579</v>
       </c>
       <c r="G16" t="n">
         <v>3.524868830012078</v>
@@ -759,19 +759,19 @@
         <v>39203</v>
       </c>
       <c r="B17" t="n">
-        <v>0.1082821413043478</v>
+        <v>0.1207457065217391</v>
       </c>
       <c r="C17" t="n">
-        <v>3.434029499693251</v>
+        <v>3.927217963141789</v>
       </c>
       <c r="D17" t="n">
-        <v>5.193541612621352</v>
+        <v>5.003098338917025</v>
       </c>
       <c r="E17" t="n">
         <v>0.103757</v>
       </c>
       <c r="F17" t="n">
-        <v>0.004525141304347835</v>
+        <v>0.01698870652173914</v>
       </c>
       <c r="G17" t="n">
         <v>3.89059864520764</v>
@@ -782,19 +782,19 @@
         <v>39234</v>
       </c>
       <c r="B18" t="n">
-        <v>-0.1537200752688172</v>
+        <v>-0.1515090531914894</v>
       </c>
       <c r="C18" t="n">
-        <v>0.1349486253825868</v>
+        <v>0.1392408142714966</v>
       </c>
       <c r="D18" t="n">
-        <v>4.395190005017463</v>
+        <v>4.245083646563793</v>
       </c>
       <c r="E18" t="n">
         <v>-0.041719</v>
       </c>
       <c r="F18" t="n">
-        <v>-0.1120010752688172</v>
+        <v>-0.1097900531914894</v>
       </c>
       <c r="G18" t="n">
         <v>3.728286760328223</v>
@@ -805,19 +805,19 @@
         <v>39264</v>
       </c>
       <c r="B19" t="n">
-        <v>0.2330484623655914</v>
+        <v>0.2389452608695652</v>
       </c>
       <c r="C19" t="n">
-        <v>12.35269594151695</v>
+        <v>13.08053253627619</v>
       </c>
       <c r="D19" t="n">
-        <v>5.419482277491398</v>
+        <v>5.259426265905104</v>
       </c>
       <c r="E19" t="n">
         <v>0.185033</v>
       </c>
       <c r="F19" t="n">
-        <v>0.04801546236559137</v>
+        <v>0.05391226086956524</v>
       </c>
       <c r="G19" t="n">
         <v>4.418142844452035</v>
@@ -828,19 +828,19 @@
         <v>39295</v>
       </c>
       <c r="B20" t="n">
-        <v>0.1267687362637363</v>
+        <v>0.1198067634408602</v>
       </c>
       <c r="C20" t="n">
-        <v>4.188104029015912</v>
+        <v>3.887917446020487</v>
       </c>
       <c r="D20" t="n">
-        <v>6.106503197012698</v>
+        <v>5.889541104379043</v>
       </c>
       <c r="E20" t="n">
         <v>0.187476</v>
       </c>
       <c r="F20" t="n">
-        <v>-0.06070726373626373</v>
+        <v>-0.06766923655913978</v>
       </c>
       <c r="G20" t="n">
         <v>5.246438592358524</v>
@@ -851,19 +851,19 @@
         <v>39326</v>
       </c>
       <c r="B21" t="n">
-        <v>0.07019934831460675</v>
+        <v>0.06363893333333334</v>
       </c>
       <c r="C21" t="n">
-        <v>2.25723193592746</v>
+        <v>2.096673035170947</v>
       </c>
       <c r="D21" t="n">
-        <v>6.535175741924053</v>
+        <v>6.264345218084547</v>
       </c>
       <c r="E21" t="n">
         <v>0.053617</v>
       </c>
       <c r="F21" t="n">
-        <v>0.01658234831460675</v>
+        <v>0.01002193333333334</v>
       </c>
       <c r="G21" t="n">
         <v>5.527736890365012</v>
@@ -874,19 +874,19 @@
         <v>39356</v>
       </c>
       <c r="B22" t="n">
-        <v>-0.1005402988505748</v>
+        <v>-0.118000808988764</v>
       </c>
       <c r="C22" t="n">
-        <v>0.2804016229588213</v>
+        <v>0.2216247411928405</v>
       </c>
       <c r="D22" t="n">
-        <v>5.878127219789981</v>
+        <v>5.525147414565675</v>
       </c>
       <c r="E22" t="n">
         <v>0.019304</v>
       </c>
       <c r="F22" t="n">
-        <v>-0.1198442988505748</v>
+        <v>-0.137304808988764</v>
       </c>
       <c r="G22" t="n">
         <v>5.634444323296618</v>
@@ -897,19 +897,19 @@
         <v>39387</v>
       </c>
       <c r="B23" t="n">
-        <v>-0.05694751724137931</v>
+        <v>-0.0540322888888889</v>
       </c>
       <c r="C23" t="n">
-        <v>0.4948007545145409</v>
+        <v>0.5134708028329443</v>
       </c>
       <c r="D23" t="n">
-        <v>5.54338246859397</v>
+        <v>5.226611053308164</v>
       </c>
       <c r="E23" t="n">
         <v>-0.167201</v>
       </c>
       <c r="F23" t="n">
-        <v>0.1102534827586207</v>
+        <v>0.1131687111111111</v>
       </c>
       <c r="G23" t="n">
         <v>4.6923595979971</v>
@@ -920,19 +920,19 @@
         <v>39417</v>
       </c>
       <c r="B24" t="n">
-        <v>0.2045107209302326</v>
+        <v>0.211452415730337</v>
       </c>
       <c r="C24" t="n">
-        <v>9.326700658682535</v>
+        <v>9.992549848803968</v>
       </c>
       <c r="D24" t="n">
-        <v>6.677063613638135</v>
+        <v>6.331790586613057</v>
       </c>
       <c r="E24" t="n">
         <v>0.126835</v>
       </c>
       <c r="F24" t="n">
-        <v>0.07767572093023262</v>
+        <v>0.08461741573033704</v>
       </c>
       <c r="G24" t="n">
         <v>5.287515027609063</v>
@@ -943,19 +943,19 @@
         <v>39448</v>
       </c>
       <c r="B25" t="n">
-        <v>-0.07437182022471911</v>
+        <v>-0.07395647191011237</v>
       </c>
       <c r="C25" t="n">
-        <v>0.3955840872812063</v>
+        <v>0.3977194322551485</v>
       </c>
       <c r="D25" t="n">
-        <v>6.180478238935627</v>
+        <v>5.863513693953494</v>
       </c>
       <c r="E25" t="n">
         <v>-0.134478</v>
       </c>
       <c r="F25" t="n">
-        <v>0.06010617977528088</v>
+        <v>0.06052152808988762</v>
       </c>
       <c r="G25" t="n">
         <v>4.576460581726251</v>
@@ -966,19 +966,19 @@
         <v>39479</v>
       </c>
       <c r="B26" t="n">
-        <v>0.1034386923076923</v>
+        <v>0.08660154945054943</v>
       </c>
       <c r="C26" t="n">
-        <v>3.258205723042003</v>
+        <v>2.709217297753401</v>
       </c>
       <c r="D26" t="n">
-        <v>6.819778825807276</v>
+        <v>6.371303065074382</v>
       </c>
       <c r="E26" t="n">
         <v>0.01172</v>
       </c>
       <c r="F26" t="n">
-        <v>0.09171869230769232</v>
+        <v>0.07488154945054944</v>
       </c>
       <c r="G26" t="n">
         <v>4.630096699744082</v>
@@ -989,19 +989,19 @@
         <v>39508</v>
       </c>
       <c r="B27" t="n">
-        <v>-0.1941225795454546</v>
+        <v>-0.1980621011235955</v>
       </c>
       <c r="C27" t="n">
-        <v>0.07502877426650338</v>
+        <v>0.07074387750510601</v>
       </c>
       <c r="D27" t="n">
-        <v>5.495905768212096</v>
+        <v>5.109389393110546</v>
       </c>
       <c r="E27" t="n">
         <v>-0.189113</v>
       </c>
       <c r="F27" t="n">
-        <v>-0.005009579545454584</v>
+        <v>-0.00894910112359551</v>
       </c>
       <c r="G27" t="n">
         <v>3.75448522256538</v>
@@ -1012,19 +1012,19 @@
         <v>39539</v>
       </c>
       <c r="B28" t="n">
-        <v>-0.04215254022988506</v>
+        <v>-0.04590071428571429</v>
       </c>
       <c r="C28" t="n">
-        <v>0.5964255254228995</v>
+        <v>0.5690138646369339</v>
       </c>
       <c r="D28" t="n">
-        <v>5.264239379217878</v>
+        <v>4.87486477040292</v>
       </c>
       <c r="E28" t="n">
         <v>0.044477</v>
       </c>
       <c r="F28" t="n">
-        <v>-0.08662954022988506</v>
+        <v>-0.09037771428571428</v>
       </c>
       <c r="G28" t="n">
         <v>3.921473461809421</v>
@@ -1035,19 +1035,19 @@
         <v>39569</v>
       </c>
       <c r="B29" t="n">
-        <v>-0.02787063043478261</v>
+        <v>-0.03378185714285715</v>
       </c>
       <c r="C29" t="n">
-        <v>0.7123423564588345</v>
+        <v>0.6620674804653229</v>
       </c>
       <c r="D29" t="n">
-        <v>5.117521708959467</v>
+        <v>4.710182785138421</v>
       </c>
       <c r="E29" t="n">
         <v>-0.08784500000000001</v>
       </c>
       <c r="F29" t="n">
-        <v>0.05997436956521739</v>
+        <v>0.05406314285714286</v>
       </c>
       <c r="G29" t="n">
         <v>3.576991625556772</v>
@@ -1058,19 +1058,19 @@
         <v>39600</v>
       </c>
       <c r="B30" t="n">
-        <v>-0.2509040869565217</v>
+        <v>-0.2544749782608696</v>
       </c>
       <c r="C30" t="n">
-        <v>0.03122116694762298</v>
+        <v>0.0294813039877995</v>
       </c>
       <c r="D30" t="n">
-        <v>3.833514597092813</v>
+        <v>3.511559123285599</v>
       </c>
       <c r="E30" t="n">
         <v>-0.226927</v>
       </c>
       <c r="F30" t="n">
-        <v>-0.02397708695652173</v>
+        <v>-0.02754797826086958</v>
       </c>
       <c r="G30" t="n">
         <v>2.765275646944051</v>
@@ -1081,19 +1081,19 @@
         <v>39630</v>
       </c>
       <c r="B31" t="n">
-        <v>0.08315649462365592</v>
+        <v>0.09196028260869567</v>
       </c>
       <c r="C31" t="n">
-        <v>2.607921394346168</v>
+        <v>2.873969183495684</v>
       </c>
       <c r="D31" t="n">
-        <v>4.152296233075668</v>
+        <v>3.834483092660086</v>
       </c>
       <c r="E31" t="n">
         <v>0.004796</v>
       </c>
       <c r="F31" t="n">
-        <v>0.07836049462365592</v>
+        <v>0.08716428260869567</v>
       </c>
       <c r="G31" t="n">
         <v>2.778537908946794</v>
@@ -1104,19 +1104,19 @@
         <v>39661</v>
       </c>
       <c r="B32" t="n">
-        <v>-0.2263395434782608</v>
+        <v>-0.2324614731182795</v>
       </c>
       <c r="C32" t="n">
-        <v>0.04598379350424538</v>
+        <v>0.04180249573436771</v>
       </c>
       <c r="D32" t="n">
-        <v>3.212467399294819</v>
+        <v>2.943113504293187</v>
       </c>
       <c r="E32" t="n">
         <v>-0.147429</v>
       </c>
       <c r="F32" t="n">
-        <v>-0.07891054347826082</v>
+        <v>-0.08503247311827952</v>
       </c>
       <c r="G32" t="n">
         <v>2.368900843568677</v>
@@ -1127,19 +1127,19 @@
         <v>39692</v>
       </c>
       <c r="B33" t="n">
-        <v>-0.08210339560439561</v>
+        <v>-0.05783309677419356</v>
       </c>
       <c r="C33" t="n">
-        <v>0.357705122203623</v>
+        <v>0.4892537120741418</v>
       </c>
       <c r="D33" t="n">
-        <v>2.948712917544293</v>
+        <v>2.772904136181963</v>
       </c>
       <c r="E33" t="n">
         <v>-0.061874</v>
       </c>
       <c r="F33" t="n">
-        <v>-0.02022939560439561</v>
+        <v>0.004040903225806435</v>
       </c>
       <c r="G33" t="n">
         <v>2.222327472773709</v>
@@ -1150,19 +1150,19 @@
         <v>39722</v>
       </c>
       <c r="B34" t="n">
-        <v>-0.2454161521739131</v>
+        <v>-0.2582760543478261</v>
       </c>
       <c r="C34" t="n">
-        <v>0.03407925220679572</v>
+        <v>0.02772730111732406</v>
       </c>
       <c r="D34" t="n">
-        <v>2.225051139455059</v>
+        <v>2.056729396804118</v>
       </c>
       <c r="E34" t="n">
         <v>-0.258506</v>
       </c>
       <c r="F34" t="n">
-        <v>0.01308984782608694</v>
+        <v>0.0002299456521739351</v>
       </c>
       <c r="G34" t="n">
         <v>1.647842487096869</v>
@@ -1173,19 +1173,19 @@
         <v>39753</v>
       </c>
       <c r="B35" t="n">
-        <v>0.2131039560439561</v>
+        <v>0.2188281630434782</v>
       </c>
       <c r="C35" t="n">
-        <v>10.15725201607878</v>
+        <v>10.74755729769886</v>
       </c>
       <c r="D35" t="n">
-        <v>2.699218339673044</v>
+        <v>2.506799712584284</v>
       </c>
       <c r="E35" t="n">
         <v>0.099936</v>
       </c>
       <c r="F35" t="n">
-        <v>0.1131679560439561</v>
+        <v>0.1188921630434782</v>
       </c>
       <c r="G35" t="n">
         <v>1.812521273887381</v>
@@ -1196,19 +1196,19 @@
         <v>39783</v>
       </c>
       <c r="B36" t="n">
-        <v>0.03623676086956521</v>
+        <v>0.0576398817204301</v>
       </c>
       <c r="C36" t="n">
-        <v>1.532879230011126</v>
+        <v>1.959087470573492</v>
       </c>
       <c r="D36" t="n">
-        <v>2.797029269182522</v>
+        <v>2.651291351514451</v>
       </c>
       <c r="E36" t="n">
         <v>-0.006667</v>
       </c>
       <c r="F36" t="n">
-        <v>0.04290376086956521</v>
+        <v>0.0643068817204301</v>
       </c>
       <c r="G36" t="n">
         <v>1.800437194554374</v>
@@ -1219,19 +1219,19 @@
         <v>39814</v>
       </c>
       <c r="B37" t="n">
-        <v>0.1597652391304348</v>
+        <v>0.1494136129032258</v>
       </c>
       <c r="C37" t="n">
-        <v>5.921627075219429</v>
+        <v>5.317604532445364</v>
       </c>
       <c r="D37" t="n">
-        <v>3.243897319228292</v>
+        <v>3.047430371203301</v>
       </c>
       <c r="E37" t="n">
         <v>0.118258</v>
       </c>
       <c r="F37" t="n">
-        <v>0.04150723913043482</v>
+        <v>0.03115561290322581</v>
       </c>
       <c r="G37" t="n">
         <v>2.013353296307985</v>
@@ -1242,19 +1242,19 @@
         <v>39845</v>
       </c>
       <c r="B38" t="n">
-        <v>0.0944667659574468</v>
+        <v>0.08792094623655912</v>
       </c>
       <c r="C38" t="n">
-        <v>2.954139110270164</v>
+        <v>2.748957731248009</v>
       </c>
       <c r="D38" t="n">
-        <v>3.55033780807382</v>
+        <v>3.315363333029524</v>
       </c>
       <c r="E38" t="n">
         <v>0.053038</v>
       </c>
       <c r="F38" t="n">
-        <v>0.04142876595744679</v>
+        <v>0.03488294623655912</v>
       </c>
       <c r="G38" t="n">
         <v>2.120137528437568</v>
@@ -1265,19 +1265,19 @@
         <v>39873</v>
       </c>
       <c r="B39" t="n">
-        <v>0.2082677234042553</v>
+        <v>0.2237917934782609</v>
       </c>
       <c r="C39" t="n">
-        <v>9.681844237106832</v>
+        <v>11.28471093585745</v>
       </c>
       <c r="D39" t="n">
-        <v>4.289758580677409</v>
+        <v>4.057314439360265</v>
       </c>
       <c r="E39" t="n">
         <v>0.171596</v>
       </c>
       <c r="F39" t="n">
-        <v>0.03667172340425531</v>
+        <v>0.05219579347826087</v>
       </c>
       <c r="G39" t="n">
         <v>2.483944647767341</v>
@@ -1288,19 +1288,19 @@
         <v>39904</v>
       </c>
       <c r="B40" t="n">
-        <v>0.07488254736842104</v>
+        <v>0.07485646739130435</v>
       </c>
       <c r="C40" t="n">
-        <v>2.37865872567557</v>
+        <v>2.377966254623504</v>
       </c>
       <c r="D40" t="n">
-        <v>4.610986630794075</v>
+        <v>4.361030665386505</v>
       </c>
       <c r="E40" t="n">
         <v>0.045913</v>
       </c>
       <c r="F40" t="n">
-        <v>0.02896954736842104</v>
+        <v>0.02894346739130434</v>
       </c>
       <c r="G40" t="n">
         <v>2.597989998380283</v>
@@ -1311,19 +1311,19 @@
         <v>39934</v>
       </c>
       <c r="B41" t="n">
-        <v>0.07362951578947367</v>
+        <v>0.07503141304347827</v>
       </c>
       <c r="C41" t="n">
-        <v>2.345596523369202</v>
+        <v>2.382614921504898</v>
       </c>
       <c r="D41" t="n">
-        <v>4.95049134373118</v>
+        <v>4.688244958536394</v>
       </c>
       <c r="E41" t="n">
         <v>0.052148</v>
       </c>
       <c r="F41" t="n">
-        <v>0.02148151578947367</v>
+        <v>0.02288341304347827</v>
       </c>
       <c r="G41" t="n">
         <v>2.733469980815819</v>
@@ -1334,19 +1334,19 @@
         <v>39965</v>
       </c>
       <c r="B42" t="n">
-        <v>0.06973501063829787</v>
+        <v>0.07912694623655914</v>
       </c>
       <c r="C42" t="n">
-        <v>2.245507537654697</v>
+        <v>2.493850678689916</v>
       </c>
       <c r="D42" t="n">
-        <v>5.295713910251076</v>
+        <v>5.059211465314323</v>
       </c>
       <c r="E42" t="n">
         <v>0.147392</v>
       </c>
       <c r="F42" t="n">
-        <v>-0.07765698936170212</v>
+        <v>-0.06826505376344086</v>
       </c>
       <c r="G42" t="n">
         <v>3.136361588228224</v>
@@ -1357,19 +1357,19 @@
         <v>39995</v>
       </c>
       <c r="B43" t="n">
-        <v>0.135666914893617</v>
+        <v>0.1150796666666667</v>
       </c>
       <c r="C43" t="n">
-        <v>4.602689575763747</v>
+        <v>3.695479172871939</v>
       </c>
       <c r="D43" t="n">
-        <v>6.014167078614052</v>
+        <v>5.641423834338874</v>
       </c>
       <c r="E43" t="n">
         <v>0.179427</v>
       </c>
       <c r="F43" t="n">
-        <v>-0.04376008510638299</v>
+        <v>-0.06434733333333334</v>
       </c>
       <c r="G43" t="n">
         <v>3.699109538919249</v>
@@ -1380,19 +1380,19 @@
         <v>40026</v>
       </c>
       <c r="B44" t="n">
-        <v>-0.1415386702127659</v>
+        <v>-0.1544264516129032</v>
       </c>
       <c r="C44" t="n">
-        <v>0.160194957190737</v>
+        <v>0.1336031398010115</v>
       </c>
       <c r="D44" t="n">
-        <v>5.162929867869623</v>
+        <v>4.770238769557463</v>
       </c>
       <c r="E44" t="n">
         <v>-0.242153</v>
       </c>
       <c r="F44" t="n">
-        <v>0.1006143297872341</v>
+        <v>0.08772654838709679</v>
       </c>
       <c r="G44" t="n">
         <v>2.803359066741336</v>
@@ -1403,19 +1403,19 @@
         <v>40057</v>
       </c>
       <c r="B45" t="n">
-        <v>0.02430146808510638</v>
+        <v>0.147323752688172</v>
       </c>
       <c r="C45" t="n">
-        <v>1.333931542346684</v>
+        <v>5.202736331237533</v>
       </c>
       <c r="D45" t="n">
-        <v>5.2883966432793</v>
+        <v>5.473008246307277</v>
       </c>
       <c r="E45" t="n">
         <v>0.06166900000000001</v>
       </c>
       <c r="F45" t="n">
-        <v>-0.03736753191489363</v>
+        <v>0.08565475268817202</v>
       </c>
       <c r="G45" t="n">
         <v>2.976239417028207</v>
@@ -1426,19 +1426,19 @@
         <v>40087</v>
       </c>
       <c r="B46" t="n">
-        <v>0.1301681489361702</v>
+        <v>0.1299015376344086</v>
       </c>
       <c r="C46" t="n">
-        <v>4.342269389558432</v>
+        <v>4.329993016050723</v>
       </c>
       <c r="D46" t="n">
-        <v>5.976777445175221</v>
+        <v>6.18396043298839</v>
       </c>
       <c r="E46" t="n">
         <v>0.091706</v>
       </c>
       <c r="F46" t="n">
-        <v>0.03846214893617021</v>
+        <v>0.03819553763440865</v>
       </c>
       <c r="G46" t="n">
         <v>3.249178429006196</v>
@@ -1449,19 +1449,19 @@
         <v>40118</v>
       </c>
       <c r="B47" t="n">
-        <v>0.1405621063829788</v>
+        <v>0.1604080215053764</v>
       </c>
       <c r="C47" t="n">
-        <v>4.846489361739926</v>
+        <v>5.961131019109101</v>
       </c>
       <c r="D47" t="n">
-        <v>6.816885872251329</v>
+        <v>7.175917291111589</v>
       </c>
       <c r="E47" t="n">
         <v>0.07051</v>
       </c>
       <c r="F47" t="n">
-        <v>0.07005210638297875</v>
+        <v>0.08989802150537636</v>
       </c>
       <c r="G47" t="n">
         <v>3.478278000035423</v>
@@ -1472,19 +1472,19 @@
         <v>40148</v>
       </c>
       <c r="B48" t="n">
-        <v>0.01058156382978723</v>
+        <v>0.04418543010752689</v>
       </c>
       <c r="C48" t="n">
-        <v>1.134635723491111</v>
+        <v>1.680086138153919</v>
       </c>
       <c r="D48" t="n">
-        <v>6.889019185228931</v>
+        <v>7.492988283035394</v>
       </c>
       <c r="E48" t="n">
         <v>0.018228</v>
       </c>
       <c r="F48" t="n">
-        <v>-0.007646436170212767</v>
+        <v>0.02595743010752689</v>
       </c>
       <c r="G48" t="n">
         <v>3.541680051420069</v>
@@ -1495,19 +1495,19 @@
         <v>40179</v>
       </c>
       <c r="B49" t="n">
-        <v>-0.03414813829787233</v>
+        <v>-0.01978903225806452</v>
       </c>
       <c r="C49" t="n">
-        <v>0.659061974499957</v>
+        <v>0.7867462674187498</v>
       </c>
       <c r="D49" t="n">
-        <v>6.653772005355038</v>
+        <v>7.344709296193107</v>
       </c>
       <c r="E49" t="n">
         <v>-0.103902</v>
       </c>
       <c r="F49" t="n">
-        <v>0.06975386170212766</v>
+        <v>0.08411296774193547</v>
       </c>
       <c r="G49" t="n">
         <v>3.173692410717421</v>
@@ -1518,19 +1518,19 @@
         <v>40210</v>
       </c>
       <c r="B50" t="n">
-        <v>0.07320986170212766</v>
+        <v>0.07020451612903225</v>
       </c>
       <c r="C50" t="n">
-        <v>2.334618146546884</v>
+        <v>2.257362736966593</v>
       </c>
       <c r="D50" t="n">
-        <v>7.140893733664569</v>
+        <v>7.86034105844075</v>
       </c>
       <c r="E50" t="n">
         <v>0.02419</v>
       </c>
       <c r="F50" t="n">
-        <v>0.04901986170212766</v>
+        <v>0.04601451612903225</v>
       </c>
       <c r="G50" t="n">
         <v>3.250464030132675</v>
@@ -1541,19 +1541,19 @@
         <v>40238</v>
       </c>
       <c r="B51" t="n">
-        <v>0.03142856382978723</v>
+        <v>0.03044998924731182</v>
       </c>
       <c r="C51" t="n">
-        <v>1.449672338989687</v>
+        <v>1.43325355790261</v>
       </c>
       <c r="D51" t="n">
-        <v>7.365321768174774</v>
+        <v>8.099688359150475</v>
       </c>
       <c r="E51" t="n">
         <v>0.019484</v>
       </c>
       <c r="F51" t="n">
-        <v>0.01194456382978723</v>
+        <v>0.01096598924731182</v>
       </c>
       <c r="G51" t="n">
         <v>3.31379607129578</v>
@@ -1564,19 +1564,19 @@
         <v>40269</v>
       </c>
       <c r="B52" t="n">
-        <v>-0.07649520212765958</v>
+        <v>-0.06415093548387096</v>
       </c>
       <c r="C52" t="n">
-        <v>0.3848308436028112</v>
+        <v>0.4513045652615694</v>
       </c>
       <c r="D52" t="n">
-        <v>6.801909990782994</v>
+        <v>7.580085773783153</v>
       </c>
       <c r="E52" t="n">
         <v>-0.08316599999999999</v>
       </c>
       <c r="F52" t="n">
-        <v>0.006670797872340414</v>
+        <v>0.01901506451612903</v>
       </c>
       <c r="G52" t="n">
         <v>3.038200907230395</v>
@@ -1587,19 +1587,19 @@
         <v>40299</v>
       </c>
       <c r="B53" t="n">
-        <v>-0.08221304255319146</v>
+        <v>-0.06860908695652172</v>
       </c>
       <c r="C53" t="n">
-        <v>0.3571927047887969</v>
+        <v>0.4261710631658803</v>
       </c>
       <c r="D53" t="n">
-        <v>6.242704275267773</v>
+        <v>7.060023009791771</v>
       </c>
       <c r="E53" t="n">
         <v>-0.09588300000000001</v>
       </c>
       <c r="F53" t="n">
-        <v>0.01366995744680854</v>
+        <v>0.02727391304347829</v>
       </c>
       <c r="G53" t="n">
         <v>2.746889089642423</v>
@@ -1610,19 +1610,19 @@
         <v>40330</v>
       </c>
       <c r="B54" t="n">
-        <v>-0.09642592473118278</v>
+        <v>-0.09765972826086955</v>
       </c>
       <c r="C54" t="n">
-        <v>0.2961864206109611</v>
+        <v>0.2913694982193021</v>
       </c>
       <c r="D54" t="n">
-        <v>5.64074574270177</v>
+        <v>6.370543081140021</v>
       </c>
       <c r="E54" t="n">
         <v>-0.075792</v>
       </c>
       <c r="F54" t="n">
-        <v>-0.02063392473118278</v>
+        <v>-0.02186772826086955</v>
       </c>
       <c r="G54" t="n">
         <v>2.538696871760245</v>
@@ -1633,19 +1633,19 @@
         <v>40360</v>
       </c>
       <c r="B55" t="n">
-        <v>0.03570829032258065</v>
+        <v>0.1450156582278481</v>
       </c>
       <c r="C55" t="n">
-        <v>1.523524458833781</v>
+        <v>5.078519319935174</v>
       </c>
       <c r="D55" t="n">
-        <v>5.842167129318026</v>
+        <v>7.294371579320404</v>
       </c>
       <c r="E55" t="n">
         <v>0.119302</v>
       </c>
       <c r="F55" t="n">
-        <v>-0.08359370967741934</v>
+        <v>0.0257136582278481</v>
       </c>
       <c r="G55" t="n">
         <v>2.841568485954986</v>
@@ -1656,19 +1656,19 @@
         <v>40391</v>
       </c>
       <c r="B56" t="n">
-        <v>0.08781745161290323</v>
+        <v>0.1074041265822785</v>
       </c>
       <c r="C56" t="n">
-        <v>2.745821251115587</v>
+        <v>3.4015248665389</v>
       </c>
       <c r="D56" t="n">
-        <v>6.355211358511407</v>
+        <v>8.077817187763907</v>
       </c>
       <c r="E56" t="n">
         <v>0.01197</v>
       </c>
       <c r="F56" t="n">
-        <v>0.07584745161290324</v>
+        <v>0.09543412658227848</v>
       </c>
       <c r="G56" t="n">
         <v>2.875582060731867</v>
@@ -1679,19 +1679,19 @@
         <v>40422</v>
       </c>
       <c r="B57" t="n">
-        <v>-0.01181049462365591</v>
+        <v>0.02404220652173913</v>
       </c>
       <c r="C57" t="n">
-        <v>0.8671272774954398</v>
+        <v>1.329885591216029</v>
       </c>
       <c r="D57" t="n">
-        <v>6.280153168929511</v>
+        <v>8.272025736836982</v>
       </c>
       <c r="E57" t="n">
         <v>0.011153</v>
       </c>
       <c r="F57" t="n">
-        <v>-0.02296349462365591</v>
+        <v>0.01288920652173913</v>
       </c>
       <c r="G57" t="n">
         <v>2.90765342745521</v>
@@ -1702,19 +1702,19 @@
         <v>40452</v>
       </c>
       <c r="B58" t="n">
-        <v>-0.01298882608695652</v>
+        <v>0.06590232608695654</v>
       </c>
       <c r="C58" t="n">
-        <v>0.8548006267655792</v>
+        <v>2.15084403565871</v>
       </c>
       <c r="D58" t="n">
-        <v>6.198581351618836</v>
+        <v>8.817171474345709</v>
       </c>
       <c r="E58" t="n">
         <v>0.151388</v>
       </c>
       <c r="F58" t="n">
-        <v>-0.1643768260869565</v>
+        <v>-0.08548567391304349</v>
       </c>
       <c r="G58" t="n">
         <v>3.347837264530799</v>
@@ -1725,19 +1725,19 @@
         <v>40483</v>
       </c>
       <c r="B59" t="n">
-        <v>-0.03615959782608695</v>
+        <v>0.0312386847826087</v>
       </c>
       <c r="C59" t="n">
-        <v>0.6427787707585321</v>
+        <v>1.44647308068362</v>
       </c>
       <c r="D59" t="n">
-        <v>5.974443142852017</v>
+        <v>9.092608314707004</v>
       </c>
       <c r="E59" t="n">
         <v>-0.071891</v>
       </c>
       <c r="F59" t="n">
-        <v>0.03573140217391305</v>
+        <v>0.1031296847826087</v>
       </c>
       <c r="G59" t="n">
         <v>3.107157895746415</v>
@@ -1748,19 +1748,19 @@
         <v>40513</v>
       </c>
       <c r="B60" t="n">
-        <v>0.1103950217391304</v>
+        <v>-0.02423859782608696</v>
       </c>
       <c r="C60" t="n">
-        <v>3.513420026008172</v>
+        <v>0.7449439865301858</v>
       </c>
       <c r="D60" t="n">
-        <v>6.633991923486365</v>
+        <v>8.872216238576687</v>
       </c>
       <c r="E60" t="n">
         <v>-0.002783</v>
       </c>
       <c r="F60" t="n">
-        <v>0.1131780217391304</v>
+        <v>-0.02145559782608696</v>
       </c>
       <c r="G60" t="n">
         <v>3.098510675322553</v>
@@ -1771,19 +1771,19 @@
         <v>40544</v>
       </c>
       <c r="B61" t="n">
-        <v>0.02995930434782609</v>
+        <v>-0.0402511978021978</v>
       </c>
       <c r="C61" t="n">
-        <v>1.425085046122027</v>
+        <v>0.6107886318876232</v>
       </c>
       <c r="D61" t="n">
-        <v>6.832741706563113</v>
+        <v>8.515098907813865</v>
       </c>
       <c r="E61" t="n">
         <v>-0.016543</v>
       </c>
       <c r="F61" t="n">
-        <v>0.0465023043478261</v>
+        <v>-0.0237081978021978</v>
       </c>
       <c r="G61" t="n">
         <v>3.047252013220692</v>
@@ -1794,19 +1794,19 @@
         <v>40575</v>
       </c>
       <c r="B62" t="n">
-        <v>0.006605413043478264</v>
+        <v>0.1010160111111111</v>
       </c>
       <c r="C62" t="n">
-        <v>1.082208991540548</v>
+        <v>3.173391213891961</v>
       </c>
       <c r="D62" t="n">
-        <v>6.877874787754363</v>
+        <v>9.375260233697801</v>
       </c>
       <c r="E62" t="n">
         <v>0.052998</v>
       </c>
       <c r="F62" t="n">
-        <v>-0.04639258695652174</v>
+        <v>0.04801801111111111</v>
       </c>
       <c r="G62" t="n">
         <v>3.208750275417363</v>
@@ -1817,19 +1817,19 @@
         <v>40603</v>
       </c>
       <c r="B63" t="n">
-        <v>-0.05910536956521738</v>
+        <v>-0.0212563</v>
       </c>
       <c r="C63" t="n">
-        <v>0.4813842544971078</v>
+        <v>0.7727299676559714</v>
       </c>
       <c r="D63" t="n">
-        <v>6.47135545660085</v>
+        <v>9.175976889592251</v>
       </c>
       <c r="E63" t="n">
         <v>-0.005022</v>
       </c>
       <c r="F63" t="n">
-        <v>-0.05408336956521739</v>
+        <v>-0.0162343</v>
       </c>
       <c r="G63" t="n">
         <v>3.192635931534217</v>
@@ -1840,19 +1840,19 @@
         <v>40634</v>
       </c>
       <c r="B64" t="n">
-        <v>0.01350566304347826</v>
+        <v>-0.03372363333333334</v>
       </c>
       <c r="C64" t="n">
-        <v>1.174665344761752</v>
+        <v>0.6625463893280207</v>
       </c>
       <c r="D64" t="n">
-        <v>6.558755402832276</v>
+        <v>8.866529609492503</v>
       </c>
       <c r="E64" t="n">
         <v>-0.009484000000000001</v>
       </c>
       <c r="F64" t="n">
-        <v>0.02298966304347826</v>
+        <v>-0.02423963333333334</v>
       </c>
       <c r="G64" t="n">
         <v>3.162356972359546</v>
@@ -1863,19 +1863,19 @@
         <v>40664</v>
       </c>
       <c r="B65" t="n">
-        <v>0.01114503191489362</v>
+        <v>-0.07675344318181818</v>
       </c>
       <c r="C65" t="n">
-        <v>1.142250688317157</v>
+        <v>0.3835414977601029</v>
       </c>
       <c r="D65" t="n">
-        <v>6.631852941118822</v>
+        <v>8.185992932890411</v>
       </c>
       <c r="E65" t="n">
         <v>-0.059874</v>
       </c>
       <c r="F65" t="n">
-        <v>0.07101903191489362</v>
+        <v>-0.01687944318181817</v>
       </c>
       <c r="G65" t="n">
         <v>2.973014010996491</v>
@@ -1886,19 +1886,19 @@
         <v>40695</v>
       </c>
       <c r="B66" t="n">
-        <v>-0.0460138085106383</v>
+        <v>0.03597330681818182</v>
       </c>
       <c r="C66" t="n">
-        <v>0.5682050149218519</v>
+        <v>1.528209111764869</v>
       </c>
       <c r="D66" t="n">
-        <v>6.326696129815468</v>
+        <v>8.480470168276746</v>
       </c>
       <c r="E66" t="n">
         <v>0.014169</v>
       </c>
       <c r="F66" t="n">
-        <v>-0.0601828085106383</v>
+        <v>0.02180430681818182</v>
       </c>
       <c r="G66" t="n">
         <v>3.015138646518301</v>
@@ -1909,19 +1909,19 @@
         <v>40725</v>
       </c>
       <c r="B67" t="n">
-        <v>-0.1164820638297872</v>
+        <v>0.01274775280898877</v>
       </c>
       <c r="C67" t="n">
-        <v>0.226247842145433</v>
+        <v>1.164167466329665</v>
       </c>
       <c r="D67" t="n">
-        <v>5.589749507390635</v>
+        <v>8.588577105685941</v>
       </c>
       <c r="E67" t="n">
         <v>-0.023656</v>
       </c>
       <c r="F67" t="n">
-        <v>-0.09282606382978725</v>
+        <v>0.03640375280898876</v>
       </c>
       <c r="G67" t="n">
         <v>2.943812526696264</v>
@@ -1932,19 +1932,19 @@
         <v>40756</v>
       </c>
       <c r="B68" t="n">
-        <v>0.0416401935483871</v>
+        <v>-0.01759835555555556</v>
       </c>
       <c r="C68" t="n">
-        <v>1.631596462016062</v>
+        <v>0.8081071868829824</v>
       </c>
       <c r="D68" t="n">
-        <v>5.822507758765382</v>
+        <v>8.437432272063775</v>
       </c>
       <c r="E68" t="n">
         <v>-0.042159</v>
       </c>
       <c r="F68" t="n">
-        <v>0.08379919354838709</v>
+        <v>0.02456064444444444</v>
       </c>
       <c r="G68" t="n">
         <v>2.819704334383276</v>
@@ -1955,19 +1955,19 @@
         <v>40787</v>
       </c>
       <c r="B69" t="n">
-        <v>-0.05360464516129032</v>
+        <v>-0.1178964239130435</v>
       </c>
       <c r="C69" t="n">
-        <v>0.5162632367316043</v>
+        <v>0.2219396990341826</v>
       </c>
       <c r="D69" t="n">
-        <v>5.510394296407903</v>
+        <v>7.442689180178951</v>
       </c>
       <c r="E69" t="n">
         <v>-0.093239</v>
       </c>
       <c r="F69" t="n">
-        <v>0.03963435483870968</v>
+        <v>-0.02465742391304347</v>
       </c>
       <c r="G69" t="n">
         <v>2.556797921949714</v>
@@ -1978,19 +1978,19 @@
         <v>40817</v>
       </c>
       <c r="B70" t="n">
-        <v>-0.1593404631578948</v>
+        <v>0.03195345652173913</v>
       </c>
       <c r="C70" t="n">
-        <v>0.1245781078131364</v>
+        <v>1.4585499967006</v>
       </c>
       <c r="D70" t="n">
-        <v>4.632365517035646</v>
+        <v>7.680508825302618</v>
       </c>
       <c r="E70" t="n">
         <v>0.04414700000000001</v>
       </c>
       <c r="F70" t="n">
-        <v>-0.2034874631578948</v>
+        <v>-0.01219354347826088</v>
       </c>
       <c r="G70" t="n">
         <v>2.669672879810028</v>
@@ -2001,19 +2001,19 @@
         <v>40848</v>
       </c>
       <c r="B71" t="n">
-        <v>0.01477857446808511</v>
+        <v>-0.03900313978494625</v>
       </c>
       <c r="C71" t="n">
-        <v>1.192491988522312</v>
+        <v>0.6203883372111518</v>
       </c>
       <c r="D71" t="n">
-        <v>4.700825275792547</v>
+        <v>7.380944865969826</v>
       </c>
       <c r="E71" t="n">
         <v>-0.06447899999999999</v>
       </c>
       <c r="F71" t="n">
-        <v>0.0792575744680851</v>
+        <v>0.02547586021505375</v>
       </c>
       <c r="G71" t="n">
         <v>2.497535042192757</v>
@@ -2024,19 +2024,19 @@
         <v>40878</v>
       </c>
       <c r="B72" t="n">
-        <v>0.1237968817204301</v>
+        <v>-0.1370517634408602</v>
       </c>
       <c r="C72" t="n">
-        <v>4.057456498692346</v>
+        <v>0.1705363435850636</v>
       </c>
       <c r="D72" t="n">
-        <v>5.282772786448245</v>
+        <v>6.369373356228897</v>
       </c>
       <c r="E72" t="n">
         <v>-0.069712</v>
       </c>
       <c r="F72" t="n">
-        <v>0.1935088817204301</v>
+        <v>-0.06733976344086021</v>
       </c>
       <c r="G72" t="n">
         <v>2.323426879331416</v>
@@ -2047,19 +2047,19 @@
         <v>40909</v>
       </c>
       <c r="B73" t="n">
-        <v>-0.06805138297872342</v>
+        <v>-0.0063055376344086</v>
       </c>
       <c r="C73" t="n">
-        <v>0.4292433921725402</v>
+        <v>0.9269033146595874</v>
       </c>
       <c r="D73" t="n">
-        <v>4.923272792368078</v>
+        <v>6.329211032823597</v>
       </c>
       <c r="E73" t="n">
         <v>0.050526</v>
       </c>
       <c r="F73" t="n">
-        <v>-0.1185773829787234</v>
+        <v>-0.0568315376344086</v>
       </c>
       <c r="G73" t="n">
         <v>2.440820345836515</v>
@@ -2070,19 +2070,19 @@
         <v>40940</v>
       </c>
       <c r="B74" t="n">
-        <v>0.08990631578947367</v>
+        <v>0.1229470217391304</v>
       </c>
       <c r="C74" t="n">
-        <v>2.809765210192045</v>
+        <v>4.020788339904193</v>
       </c>
       <c r="D74" t="n">
-        <v>5.365906110756447</v>
+        <v>7.107368679267704</v>
       </c>
       <c r="E74" t="n">
         <v>0.068938</v>
       </c>
       <c r="F74" t="n">
-        <v>0.02096831578947367</v>
+        <v>0.05400902173913043</v>
       </c>
       <c r="G74" t="n">
         <v>2.609085618837792</v>
@@ -2093,19 +2093,19 @@
         <v>40969</v>
       </c>
       <c r="B75" t="n">
-        <v>0.01328772340425532</v>
+        <v>-0.07067816304347826</v>
       </c>
       <c r="C75" t="n">
-        <v>1.171637790909537</v>
+        <v>0.4149480294162981</v>
       </c>
       <c r="D75" t="n">
-        <v>5.437206786969381</v>
+        <v>6.605032916944309</v>
       </c>
       <c r="E75" t="n">
         <v>-0.06804500000000001</v>
       </c>
       <c r="F75" t="n">
-        <v>0.08133272340425532</v>
+        <v>-0.002633163043478257</v>
       </c>
       <c r="G75" t="n">
         <v>2.431550387903975</v>
@@ -2116,19 +2116,19 @@
         <v>41000</v>
       </c>
       <c r="B76" t="n">
-        <v>-0.05732820430107528</v>
+        <v>0.07483525531914893</v>
       </c>
       <c r="C76" t="n">
-        <v>0.4924092023878104</v>
+        <v>2.37740317162219</v>
       </c>
       <c r="D76" t="n">
-        <v>5.125501485458807</v>
+        <v>7.099322241675219</v>
       </c>
       <c r="E76" t="n">
         <v>0.069762</v>
       </c>
       <c r="F76" t="n">
-        <v>-0.1270902043010753</v>
+        <v>0.005073255319148928</v>
       </c>
       <c r="G76" t="n">
         <v>2.601180206064932</v>
@@ -2139,19 +2139,19 @@
         <v>41030</v>
       </c>
       <c r="B77" t="n">
-        <v>-0.07717210752688172</v>
+        <v>0.006268106382978722</v>
       </c>
       <c r="C77" t="n">
-        <v>0.3814596018802081</v>
+        <v>1.077865311915802</v>
       </c>
       <c r="D77" t="n">
-        <v>4.729955733693788</v>
+        <v>7.143821548733087</v>
       </c>
       <c r="E77" t="n">
         <v>0.002241</v>
       </c>
       <c r="F77" t="n">
-        <v>-0.07941310752688172</v>
+        <v>0.004027106382978722</v>
       </c>
       <c r="G77" t="n">
         <v>2.607009450906723</v>
@@ -2162,19 +2162,19 @@
         <v>41061</v>
       </c>
       <c r="B78" t="n">
-        <v>0.001485031914893619</v>
+        <v>-0.0632661914893617</v>
       </c>
       <c r="C78" t="n">
-        <v>1.017966656991337</v>
+        <v>0.4564511865346169</v>
       </c>
       <c r="D78" t="n">
-        <v>4.736979868914357</v>
+        <v>6.691859166665111</v>
       </c>
       <c r="E78" t="n">
         <v>-0.064752</v>
       </c>
       <c r="F78" t="n">
-        <v>0.06623703191489362</v>
+        <v>0.001485808510638301</v>
       </c>
       <c r="G78" t="n">
         <v>2.438200374941611</v>
@@ -2185,19 +2185,19 @@
         <v>41091</v>
       </c>
       <c r="B79" t="n">
-        <v>0.006956340425531914</v>
+        <v>-0.1045887052631579</v>
       </c>
       <c r="C79" t="n">
-        <v>1.086745098430331</v>
+        <v>0.265626144954177</v>
       </c>
       <c r="D79" t="n">
-        <v>4.769931913471417</v>
+        <v>5.991966280620212</v>
       </c>
       <c r="E79" t="n">
         <v>-0.052279</v>
       </c>
       <c r="F79" t="n">
-        <v>0.05923534042553191</v>
+        <v>-0.05230970526315789</v>
       </c>
       <c r="G79" t="n">
         <v>2.310733697540039</v>
@@ -2208,19 +2208,19 @@
         <v>41122</v>
       </c>
       <c r="B80" t="n">
-        <v>0.001926989473684209</v>
+        <v>0.02818233333333334</v>
       </c>
       <c r="C80" t="n">
-        <v>1.023370531770004</v>
+        <v>1.395859312615366</v>
       </c>
       <c r="D80" t="n">
-        <v>4.779123522058867</v>
+        <v>6.160833871662744</v>
       </c>
       <c r="E80" t="n">
         <v>-0.05488999999999999</v>
       </c>
       <c r="F80" t="n">
-        <v>0.0568169894736842</v>
+        <v>0.08307233333333333</v>
       </c>
       <c r="G80" t="n">
         <v>2.183897524882066</v>
@@ -2231,19 +2231,19 @@
         <v>41153</v>
       </c>
       <c r="B81" t="n">
-        <v>-0.09663870526315789</v>
+        <v>0.0002852765957446797</v>
       </c>
       <c r="C81" t="n">
-        <v>0.2953505248849395</v>
+        <v>1.003428695520447</v>
       </c>
       <c r="D81" t="n">
-        <v>4.317275212594396</v>
+        <v>6.1625914133766</v>
       </c>
       <c r="E81" t="n">
         <v>0.04002</v>
       </c>
       <c r="F81" t="n">
-        <v>-0.1366587052631579</v>
+        <v>-0.03973472340425532</v>
       </c>
       <c r="G81" t="n">
         <v>2.271297103827846</v>
@@ -2254,19 +2254,19 @@
         <v>41183</v>
       </c>
       <c r="B82" t="n">
-        <v>0.1539994</v>
+        <v>0.006368924731182795</v>
       </c>
       <c r="C82" t="n">
-        <v>5.577852121682644</v>
+        <v>1.079161926618884</v>
       </c>
       <c r="D82" t="n">
-        <v>4.982133004968805</v>
+        <v>6.20184049423743</v>
       </c>
       <c r="E82" t="n">
         <v>-0.016696</v>
       </c>
       <c r="F82" t="n">
-        <v>0.1706954</v>
+        <v>0.0230649247311828</v>
       </c>
       <c r="G82" t="n">
         <v>2.233375527382336</v>
@@ -2277,19 +2277,19 @@
         <v>41214</v>
       </c>
       <c r="B83" t="n">
-        <v>0.06409228421052632</v>
+        <v>-0.09660378947368421</v>
       </c>
       <c r="C83" t="n">
-        <v>2.107422096381055</v>
+        <v>0.2954875410175068</v>
       </c>
       <c r="D83" t="n">
-        <v>5.301449289497909</v>
+        <v>5.602719200782748</v>
       </c>
       <c r="E83" t="n">
         <v>-0.051072</v>
       </c>
       <c r="F83" t="n">
-        <v>0.1151642842105263</v>
+        <v>-0.04553178947368421</v>
       </c>
       <c r="G83" t="n">
         <v>2.119312572447865</v>
@@ -2300,19 +2300,19 @@
         <v>41244</v>
       </c>
       <c r="B84" t="n">
-        <v>0.02222747368421053</v>
+        <v>0.1434285106382979</v>
       </c>
       <c r="C84" t="n">
-        <v>1.301878899161961</v>
+        <v>4.994686133625254</v>
       </c>
       <c r="D84" t="n">
-        <v>5.419287114068401</v>
+        <v>6.406308871275613</v>
       </c>
       <c r="E84" t="n">
         <v>0.179136</v>
       </c>
       <c r="F84" t="n">
-        <v>-0.1569085263157895</v>
+        <v>-0.03570748936170212</v>
       </c>
       <c r="G84" t="n">
         <v>2.498957749425886</v>
@@ -2323,19 +2323,19 @@
         <v>41275</v>
       </c>
       <c r="B85" t="n">
-        <v>-0.0326681489361702</v>
+        <v>0.06735220430107527</v>
       </c>
       <c r="C85" t="n">
-        <v>0.6712833181635304</v>
+        <v>2.186215736121504</v>
       </c>
       <c r="D85" t="n">
-        <v>5.242249035498146</v>
+        <v>6.837787895189559</v>
       </c>
       <c r="E85" t="n">
         <v>0.064975</v>
       </c>
       <c r="F85" t="n">
-        <v>-0.09764314893617021</v>
+        <v>0.00237720430107527</v>
       </c>
       <c r="G85" t="n">
         <v>2.661327529194833</v>
@@ -2346,19 +2346,19 @@
         <v>41306</v>
       </c>
       <c r="B86" t="n">
-        <v>-0.02197946315789474</v>
+        <v>0.03755093617021277</v>
       </c>
       <c r="C86" t="n">
-        <v>0.7659063890463388</v>
+        <v>1.556370961159961</v>
       </c>
       <c r="D86" t="n">
-        <v>5.127027215957905</v>
+        <v>7.094553231987276</v>
       </c>
       <c r="E86" t="n">
         <v>-0.005045</v>
       </c>
       <c r="F86" t="n">
-        <v>-0.01693446315789474</v>
+        <v>0.04259593617021277</v>
       </c>
       <c r="G86" t="n">
         <v>2.647901131810046</v>
@@ -2369,19 +2369,19 @@
         <v>41334</v>
       </c>
       <c r="B87" t="n">
-        <v>0.1280866736842105</v>
+        <v>-0.0200828494623656</v>
       </c>
       <c r="C87" t="n">
-        <v>4.247267614562356</v>
+        <v>0.7839210118429961</v>
       </c>
       <c r="D87" t="n">
-        <v>5.783731077938372</v>
+        <v>6.952074387426536</v>
       </c>
       <c r="E87" t="n">
         <v>-0.066675</v>
       </c>
       <c r="F87" t="n">
-        <v>0.1947616736842105</v>
+        <v>0.0465921505376344</v>
       </c>
       <c r="G87" t="n">
         <v>2.471352323846611</v>
@@ -2392,19 +2392,19 @@
         <v>41365</v>
       </c>
       <c r="B88" t="n">
-        <v>-0.1412189673913044</v>
+        <v>-0.03991904301075269</v>
       </c>
       <c r="C88" t="n">
-        <v>0.16091233108294</v>
+        <v>0.6133300842102323</v>
       </c>
       <c r="D88" t="n">
-        <v>4.966958547442919</v>
+        <v>6.674554230940904</v>
       </c>
       <c r="E88" t="n">
         <v>-0.019148</v>
       </c>
       <c r="F88" t="n">
-        <v>-0.1220709673913044</v>
+        <v>-0.02077104301075269</v>
       </c>
       <c r="G88" t="n">
         <v>2.424030869549596</v>
@@ -2415,19 +2415,19 @@
         <v>41395</v>
       </c>
       <c r="B89" t="n">
-        <v>0.04410936458333333</v>
+        <v>0.1279254130434782</v>
       </c>
       <c r="C89" t="n">
-        <v>1.678618060486112</v>
+        <v>4.239987547862714</v>
       </c>
       <c r="D89" t="n">
-        <v>5.186047932882382</v>
+        <v>7.528399337815114</v>
       </c>
       <c r="E89" t="n">
         <v>0.06501799999999999</v>
       </c>
       <c r="F89" t="n">
-        <v>-0.02090863541666666</v>
+        <v>0.06290741304347824</v>
       </c>
       <c r="G89" t="n">
         <v>2.581636508625972</v>
@@ -2438,19 +2438,19 @@
         <v>41426</v>
       </c>
       <c r="B90" t="n">
-        <v>0.09256058947368419</v>
+        <v>-0.1591236555555556</v>
       </c>
       <c r="C90" t="n">
-        <v>2.892986244029537</v>
+        <v>0.1249642021758536</v>
       </c>
       <c r="D90" t="n">
-        <v>5.666071586588758</v>
+        <v>6.33045291469995</v>
       </c>
       <c r="E90" t="n">
         <v>-0.155687</v>
       </c>
       <c r="F90" t="n">
-        <v>0.2482475894736842</v>
+        <v>-0.003436655555555584</v>
       </c>
       <c r="G90" t="n">
         <v>2.17970926550752</v>
@@ -2461,19 +2461,19 @@
         <v>41456</v>
       </c>
       <c r="B91" t="n">
-        <v>0.05999339130434782</v>
+        <v>0.06062485555555554</v>
       </c>
       <c r="C91" t="n">
-        <v>2.012045933668485</v>
+        <v>2.02647666039359</v>
       </c>
       <c r="D91" t="n">
-        <v>6.005998436441423</v>
+        <v>6.71423570825488</v>
       </c>
       <c r="E91" t="n">
         <v>-0.003462</v>
       </c>
       <c r="F91" t="n">
-        <v>0.06345539130434782</v>
+        <v>0.06408685555555554</v>
       </c>
       <c r="G91" t="n">
         <v>2.172163112030333</v>
@@ -2484,19 +2484,19 @@
         <v>41487</v>
       </c>
       <c r="B92" t="n">
-        <v>-0.01617045161290323</v>
+        <v>0.07957114444444444</v>
       </c>
       <c r="C92" t="n">
-        <v>0.8223152501735924</v>
+        <v>2.506197052284528</v>
       </c>
       <c r="D92" t="n">
-        <v>5.908878729337775</v>
+        <v>7.248495127630476</v>
       </c>
       <c r="E92" t="n">
         <v>0.055124</v>
       </c>
       <c r="F92" t="n">
-        <v>-0.07129445161290322</v>
+        <v>0.02444714444444444</v>
       </c>
       <c r="G92" t="n">
         <v>2.291901431417893</v>
@@ -2507,19 +2507,19 @@
         <v>41518</v>
       </c>
       <c r="B93" t="n">
-        <v>0.06447805376344085</v>
+        <v>0.06540304347826087</v>
       </c>
       <c r="C93" t="n">
-        <v>2.116608543252288</v>
+        <v>2.138785331529982</v>
       </c>
       <c r="D93" t="n">
-        <v>6.289871729729668</v>
+        <v>7.722568769614854</v>
       </c>
       <c r="E93" t="n">
         <v>0.041111</v>
       </c>
       <c r="F93" t="n">
-        <v>0.02336705376344084</v>
+        <v>0.02429204347826087</v>
       </c>
       <c r="G93" t="n">
         <v>2.386123791164914</v>
@@ -2530,19 +2530,19 @@
         <v>41548</v>
       </c>
       <c r="B94" t="n">
-        <v>-0.02577223157894737</v>
+        <v>-0.01484205494505495</v>
       </c>
       <c r="C94" t="n">
-        <v>0.7310145973944582</v>
+        <v>0.8357384244575752</v>
       </c>
       <c r="D94" t="n">
-        <v>6.1277676989092</v>
+        <v>7.607949979619265</v>
       </c>
       <c r="E94" t="n">
         <v>-0.014661</v>
       </c>
       <c r="F94" t="n">
-        <v>-0.01111123157894737</v>
+        <v>-0.0001810549450549457</v>
       </c>
       <c r="G94" t="n">
         <v>2.351140830262645</v>
@@ -2553,19 +2553,19 @@
         <v>41579</v>
       </c>
       <c r="B95" t="n">
-        <v>-0.00160601075268817</v>
+        <v>0.06931545555555556</v>
       </c>
       <c r="C95" t="n">
-        <v>0.9808971947938745</v>
+        <v>2.234961922293849</v>
       </c>
       <c r="D95" t="n">
-        <v>6.117926438094777</v>
+        <v>8.135298498300454</v>
       </c>
       <c r="E95" t="n">
         <v>0.027478</v>
       </c>
       <c r="F95" t="n">
-        <v>-0.02908401075268817</v>
+        <v>0.04183745555555556</v>
       </c>
       <c r="G95" t="n">
         <v>2.415745477996602</v>
@@ -2576,19 +2576,19 @@
         <v>41609</v>
       </c>
       <c r="B96" t="n">
-        <v>0.03359877419354839</v>
+        <v>-0.02603439325842696</v>
       </c>
       <c r="C96" t="n">
-        <v>1.486701662740699</v>
+        <v>0.7286575227687871</v>
       </c>
       <c r="D96" t="n">
-        <v>6.323481267021063</v>
+        <v>7.92350093792101</v>
       </c>
       <c r="E96" t="n">
         <v>-0.044658</v>
       </c>
       <c r="F96" t="n">
-        <v>0.07825677419354839</v>
+        <v>0.01862360674157303</v>
       </c>
       <c r="G96" t="n">
         <v>2.30786311644023</v>
@@ -2599,19 +2599,19 @@
         <v>41640</v>
       </c>
       <c r="B97" t="n">
-        <v>-0.01184435789473684</v>
+        <v>0.008099626373626372</v>
       </c>
       <c r="C97" t="n">
-        <v>0.866770768155158</v>
+        <v>1.101644436144408</v>
       </c>
       <c r="D97" t="n">
-        <v>6.248583691753802</v>
+        <v>7.987678335089249</v>
       </c>
       <c r="E97" t="n">
         <v>-0.054753</v>
       </c>
       <c r="F97" t="n">
-        <v>0.04290864210526316</v>
+        <v>0.06285262637362637</v>
       </c>
       <c r="G97" t="n">
         <v>2.181500687225778</v>
@@ -2622,19 +2622,19 @@
         <v>41671</v>
       </c>
       <c r="B98" t="n">
-        <v>-0.007073806451612901</v>
+        <v>0.07348876666666666</v>
       </c>
       <c r="C98" t="n">
-        <v>0.9183402326192595</v>
+        <v>2.341909187535597</v>
       </c>
       <c r="D98" t="n">
-        <v>6.204382420121631</v>
+        <v>8.57468296446501</v>
       </c>
       <c r="E98" t="n">
         <v>-0.01066</v>
       </c>
       <c r="F98" t="n">
-        <v>0.003586193548387098</v>
+        <v>0.08414876666666667</v>
       </c>
       <c r="G98" t="n">
         <v>2.158245889899951</v>
@@ -2645,19 +2645,19 @@
         <v>41699</v>
       </c>
       <c r="B99" t="n">
-        <v>0.02505273913043478</v>
+        <v>-0.0250746043956044</v>
       </c>
       <c r="C99" t="n">
-        <v>1.345719438988789</v>
+        <v>0.7373209949886356</v>
       </c>
       <c r="D99" t="n">
-        <v>6.359819194358393</v>
+        <v>8.359676181313322</v>
       </c>
       <c r="E99" t="n">
         <v>-0.014991</v>
       </c>
       <c r="F99" t="n">
-        <v>0.04004373913043478</v>
+        <v>-0.0100836043956044</v>
       </c>
       <c r="G99" t="n">
         <v>2.125891625764461</v>
@@ -2668,19 +2668,19 @@
         <v>41730</v>
       </c>
       <c r="B100" t="n">
-        <v>0.01748132258064516</v>
+        <v>-0.01779348314606741</v>
       </c>
       <c r="C100" t="n">
-        <v>1.231168087977886</v>
+        <v>0.8061831852497376</v>
       </c>
       <c r="D100" t="n">
-        <v>6.470997245249551</v>
+        <v>8.210928424074542</v>
       </c>
       <c r="E100" t="n">
         <v>0.005756</v>
       </c>
       <c r="F100" t="n">
-        <v>0.01172532258064516</v>
+        <v>-0.02354948314606741</v>
       </c>
       <c r="G100" t="n">
         <v>2.138128257962361</v>
@@ -2691,19 +2691,19 @@
         <v>41760</v>
       </c>
       <c r="B101" t="n">
-        <v>0.09423936842105265</v>
+        <v>0.01766711764705882</v>
       </c>
       <c r="C101" t="n">
-        <v>2.946782137621948</v>
+        <v>1.233868577789994</v>
       </c>
       <c r="D101" t="n">
-        <v>7.080819938696241</v>
+        <v>8.355991862534246</v>
       </c>
       <c r="E101" t="n">
         <v>-0.001017</v>
       </c>
       <c r="F101" t="n">
-        <v>0.09525636842105266</v>
+        <v>0.01868411764705882</v>
       </c>
       <c r="G101" t="n">
         <v>2.135953781524013</v>
@@ -2714,19 +2714,19 @@
         <v>41791</v>
       </c>
       <c r="B102" t="n">
-        <v>0.04123710638297873</v>
+        <v>0.02446821839080459</v>
       </c>
       <c r="C102" t="n">
-        <v>1.624035951570998</v>
+        <v>1.336539752144265</v>
       </c>
       <c r="D102" t="n">
-        <v>7.372812463786974</v>
+        <v>8.560448096298519</v>
       </c>
       <c r="E102" t="n">
         <v>0.004013</v>
       </c>
       <c r="F102" t="n">
-        <v>0.03722410638297872</v>
+        <v>0.02045521839080459</v>
       </c>
       <c r="G102" t="n">
         <v>2.144525364049269</v>
@@ -2737,19 +2737,19 @@
         <v>41821</v>
       </c>
       <c r="B103" t="n">
-        <v>0.155505</v>
+        <v>0.0752518823529412</v>
       </c>
       <c r="C103" t="n">
-        <v>5.665809245083999</v>
+        <v>2.388485109518051</v>
       </c>
       <c r="D103" t="n">
-        <v>8.519321665968167</v>
+        <v>9.204637929329634</v>
       </c>
       <c r="E103" t="n">
         <v>0.085507</v>
       </c>
       <c r="F103" t="n">
-        <v>0.069998</v>
+        <v>-0.0102551176470588</v>
       </c>
       <c r="G103" t="n">
         <v>2.32789729435303</v>
@@ -2760,19 +2760,19 @@
         <v>41852</v>
       </c>
       <c r="B104" t="n">
-        <v>0.03836881818181818</v>
+        <v>0.06947605747126435</v>
       </c>
       <c r="C104" t="n">
-        <v>1.571157256081768</v>
+        <v>2.238993314326046</v>
       </c>
       <c r="D104" t="n">
-        <v>8.846197970002125</v>
+        <v>9.844139883109918</v>
       </c>
       <c r="E104" t="n">
         <v>-0.005091</v>
       </c>
       <c r="F104" t="n">
-        <v>0.04345981818181818</v>
+        <v>0.07456705747126435</v>
       </c>
       <c r="G104" t="n">
         <v>2.316045969227479</v>
@@ -2783,19 +2783,19 @@
         <v>41883</v>
       </c>
       <c r="B105" t="n">
-        <v>0.06208626436781609</v>
+        <v>0.1532885747126437</v>
       </c>
       <c r="C105" t="n">
-        <v>2.060238541351965</v>
+        <v>5.536762253574281</v>
       </c>
       <c r="D105" t="n">
-        <v>9.395425355817716</v>
+        <v>11.35313405506373</v>
       </c>
       <c r="E105" t="n">
         <v>0.048198</v>
       </c>
       <c r="F105" t="n">
-        <v>0.01388826436781608</v>
+        <v>0.1050905747126437</v>
       </c>
       <c r="G105" t="n">
         <v>2.427674752852305</v>
@@ -2806,19 +2806,19 @@
         <v>41913</v>
       </c>
       <c r="B106" t="n">
-        <v>0.05053507865168539</v>
+        <v>0.02793394186046512</v>
       </c>
       <c r="C106" t="n">
-        <v>1.806869151551597</v>
+        <v>1.391818092826708</v>
       </c>
       <c r="D106" t="n">
-        <v>9.870223915140004</v>
+        <v>11.67027184169194</v>
       </c>
       <c r="E106" t="n">
         <v>0.023393</v>
       </c>
       <c r="F106" t="n">
-        <v>0.02714207865168539</v>
+        <v>0.004540941860465119</v>
       </c>
       <c r="G106" t="n">
         <v>2.484465348345779</v>
@@ -2829,19 +2829,19 @@
         <v>41944</v>
       </c>
       <c r="B107" t="n">
-        <v>0.04919521739130435</v>
+        <v>0.04586189285714286</v>
       </c>
       <c r="C107" t="n">
-        <v>1.779408361620336</v>
+        <v>1.712742487958236</v>
       </c>
       <c r="D107" t="n">
-        <v>10.35579172634617</v>
+        <v>12.20549259850935</v>
       </c>
       <c r="E107" t="n">
         <v>0.119799</v>
       </c>
       <c r="F107" t="n">
-        <v>-0.07060378260869565</v>
+        <v>-0.07393710714285714</v>
       </c>
       <c r="G107" t="n">
         <v>2.782101812612255</v>
@@ -2852,19 +2852,19 @@
         <v>41974</v>
       </c>
       <c r="B108" t="n">
-        <v>0.06534759550561797</v>
+        <v>-0.02445525</v>
       </c>
       <c r="C108" t="n">
-        <v>2.137449979190586</v>
+        <v>0.7429615741781843</v>
       </c>
       <c r="D108" t="n">
-        <v>11.03251781521986</v>
+        <v>11.90700422563965</v>
       </c>
       <c r="E108" t="n">
         <v>0.258075</v>
       </c>
       <c r="F108" t="n">
-        <v>-0.192727404494382</v>
+        <v>-0.28253025</v>
       </c>
       <c r="G108" t="n">
         <v>3.500092737902163</v>
@@ -2875,19 +2875,19 @@
         <v>42005</v>
       </c>
       <c r="B109" t="n">
-        <v>0.2193528988764045</v>
+        <v>0.06972272619047619</v>
       </c>
       <c r="C109" t="n">
-        <v>10.80321405181225</v>
+        <v>2.24519811809511</v>
       </c>
       <c r="D109" t="n">
-        <v>13.45253257989391</v>
+        <v>12.73719302101277</v>
       </c>
       <c r="E109" t="n">
         <v>-0.028105</v>
       </c>
       <c r="F109" t="n">
-        <v>0.2474578988764045</v>
+        <v>0.09782772619047619</v>
       </c>
       <c r="G109" t="n">
         <v>3.401722631503422</v>
@@ -2898,19 +2898,19 @@
         <v>42036</v>
       </c>
       <c r="B110" t="n">
-        <v>0.1801123222222222</v>
+        <v>0.06180636470588235</v>
       </c>
       <c r="C110" t="n">
-        <v>7.295921309302575</v>
+        <v>2.053732573083517</v>
       </c>
       <c r="D110" t="n">
-        <v>15.87549946262871</v>
+        <v>13.52443261819871</v>
       </c>
       <c r="E110" t="n">
         <v>0.040314</v>
       </c>
       <c r="F110" t="n">
-        <v>0.1397983222222222</v>
+        <v>0.02149236470588235</v>
       </c>
       <c r="G110" t="n">
         <v>3.538859677669851</v>
@@ -2921,19 +2921,19 @@
         <v>42064</v>
       </c>
       <c r="B111" t="n">
-        <v>0.2265659888888889</v>
+        <v>0.2256497469879518</v>
       </c>
       <c r="C111" t="n">
-        <v>11.59554103209387</v>
+        <v>11.4920249136719</v>
       </c>
       <c r="D111" t="n">
-        <v>19.47234769748421</v>
+        <v>16.57621741665085</v>
       </c>
       <c r="E111" t="n">
         <v>0.133888</v>
       </c>
       <c r="F111" t="n">
-        <v>0.09267798888888892</v>
+        <v>0.09176174698795181</v>
       </c>
       <c r="G111" t="n">
         <v>4.012670522193712</v>
@@ -2944,19 +2944,19 @@
         <v>42095</v>
       </c>
       <c r="B112" t="n">
-        <v>-0.06249553260869565</v>
+        <v>0.2103803373493976</v>
       </c>
       <c r="C112" t="n">
-        <v>0.4609779485034899</v>
+        <v>9.886949579930207</v>
       </c>
       <c r="D112" t="n">
-        <v>18.25541295698822</v>
+        <v>20.06352762874281</v>
       </c>
       <c r="E112" t="n">
         <v>0.172463</v>
       </c>
       <c r="F112" t="n">
-        <v>-0.2349585326086956</v>
+        <v>0.03791733734939759</v>
       </c>
       <c r="G112" t="n">
         <v>4.704707718462807</v>
@@ -2967,19 +2967,19 @@
         <v>42125</v>
       </c>
       <c r="B113" t="n">
-        <v>-0.1882109431818182</v>
+        <v>0.241962256097561</v>
       </c>
       <c r="C113" t="n">
-        <v>0.08190648922381093</v>
+        <v>13.46792754113535</v>
       </c>
       <c r="D113" t="n">
-        <v>14.81954446617988</v>
+        <v>24.91814403906917</v>
       </c>
       <c r="E113" t="n">
         <v>0.019146</v>
       </c>
       <c r="F113" t="n">
-        <v>-0.2073569431818182</v>
+        <v>0.222816256097561</v>
       </c>
       <c r="G113" t="n">
         <v>4.794784052440496</v>
@@ -2990,19 +2990,19 @@
         <v>42156</v>
       </c>
       <c r="B114" t="n">
-        <v>-0.09765626436781612</v>
+        <v>-0.06751171951219512</v>
       </c>
       <c r="C114" t="n">
-        <v>0.2913829205716699</v>
+        <v>0.4322356537754573</v>
       </c>
       <c r="D114" t="n">
-        <v>13.37232311398001</v>
+        <v>23.23587728793905</v>
       </c>
       <c r="E114" t="n">
         <v>-0.075985</v>
       </c>
       <c r="F114" t="n">
-        <v>-0.02167126436781612</v>
+        <v>0.00847328048780488</v>
       </c>
       <c r="G114" t="n">
         <v>4.430452386215805</v>
@@ -3013,19 +3013,19 @@
         <v>42186</v>
       </c>
       <c r="B115" t="n">
-        <v>-0.05859073170731707</v>
+        <v>-0.1694754634146342</v>
       </c>
       <c r="C115" t="n">
-        <v>0.4845533897839572</v>
+        <v>0.1077034488974388</v>
       </c>
       <c r="D115" t="n">
-        <v>12.58882891810526</v>
+        <v>19.29796621672001</v>
       </c>
       <c r="E115" t="n">
         <v>-0.146725</v>
       </c>
       <c r="F115" t="n">
-        <v>0.08813426829268292</v>
+        <v>-0.02275046341463416</v>
       </c>
       <c r="G115" t="n">
         <v>3.780394259848291</v>
@@ -3036,19 +3036,19 @@
         <v>42217</v>
       </c>
       <c r="B116" t="n">
-        <v>0.2107910240963856</v>
+        <v>-0.1252017710843374</v>
       </c>
       <c r="C116" t="n">
-        <v>9.927280954329689</v>
+        <v>0.2008605933670981</v>
       </c>
       <c r="D116" t="n">
-        <v>15.24244105792686</v>
+        <v>16.88182666806095</v>
       </c>
       <c r="E116" t="n">
         <v>-0.117946</v>
       </c>
       <c r="F116" t="n">
-        <v>0.3287370240963856</v>
+        <v>-0.007255771084337351</v>
       </c>
       <c r="G116" t="n">
         <v>3.334511878476225</v>
@@ -3059,19 +3059,19 @@
         <v>42248</v>
       </c>
       <c r="B117" t="n">
-        <v>0.07814431764705883</v>
+        <v>-0.057503175</v>
       </c>
       <c r="C117" t="n">
-        <v>2.46673661046896</v>
+        <v>0.4913135597804995</v>
       </c>
       <c r="D117" t="n">
-        <v>16.43355121367407</v>
+        <v>15.91106803484778</v>
       </c>
       <c r="E117" t="n">
         <v>-0.048592</v>
       </c>
       <c r="F117" t="n">
-        <v>0.1267363176470588</v>
+        <v>-0.008911174999999993</v>
       </c>
       <c r="G117" t="n">
         <v>3.172481277277308</v>
@@ -3082,19 +3082,19 @@
         <v>42278</v>
       </c>
       <c r="B118" t="n">
-        <v>0.1041313372093023</v>
+        <v>0.1973959642857143</v>
       </c>
       <c r="C118" t="n">
-        <v>3.282833323669403</v>
+        <v>8.686673149002269</v>
       </c>
       <c r="D118" t="n">
-        <v>18.1447988766515</v>
+        <v>19.05184865240216</v>
       </c>
       <c r="E118" t="n">
         <v>0.103383</v>
       </c>
       <c r="F118" t="n">
-        <v>0.0007483372093023272</v>
+        <v>0.0940129642857143</v>
       </c>
       <c r="G118" t="n">
         <v>3.500461909166068</v>
@@ -3105,19 +3105,19 @@
         <v>42309</v>
       </c>
       <c r="B119" t="n">
-        <v>-0.2675962528735632</v>
+        <v>0.08103871764705882</v>
       </c>
       <c r="C119" t="n">
-        <v>0.02382356172474928</v>
+        <v>2.547387321957481</v>
       </c>
       <c r="D119" t="n">
-        <v>13.28931868811512</v>
+        <v>20.59578603599868</v>
       </c>
       <c r="E119" t="n">
         <v>0.009148999999999999</v>
       </c>
       <c r="F119" t="n">
-        <v>-0.2767452528735632</v>
+        <v>0.07188971764705882</v>
       </c>
       <c r="G119" t="n">
         <v>3.532487635173029</v>
@@ -3128,19 +3128,19 @@
         <v>42339</v>
       </c>
       <c r="B120" t="n">
-        <v>-0.01739997674418605</v>
+        <v>0.1097295529411765</v>
       </c>
       <c r="C120" t="n">
-        <v>0.8100675603458543</v>
+        <v>3.488235690793038</v>
       </c>
       <c r="D120" t="n">
-        <v>13.05808485199584</v>
+        <v>22.85575243020094</v>
       </c>
       <c r="E120" t="n">
         <v>0.046151</v>
       </c>
       <c r="F120" t="n">
-        <v>-0.06355097674418606</v>
+        <v>0.06357855294117647</v>
       </c>
       <c r="G120" t="n">
         <v>3.6955154720239</v>
@@ -3151,19 +3151,19 @@
         <v>42370</v>
       </c>
       <c r="B121" t="n">
-        <v>0.1776187764705882</v>
+        <v>-0.3065270481927712</v>
       </c>
       <c r="C121" t="n">
-        <v>7.113063070895485</v>
+        <v>0.01236956190481713</v>
       </c>
       <c r="D121" t="n">
-        <v>15.37744590645647</v>
+        <v>15.84984610354669</v>
       </c>
       <c r="E121" t="n">
         <v>-0.210376</v>
       </c>
       <c r="F121" t="n">
-        <v>0.3879947764705883</v>
+        <v>-0.09615104819277112</v>
       </c>
       <c r="G121" t="n">
         <v>2.9180677090814</v>
@@ -3174,19 +3174,19 @@
         <v>42401</v>
       </c>
       <c r="B122" t="n">
-        <v>-0.006393287356321839</v>
+        <v>-0.01992914457831325</v>
       </c>
       <c r="C122" t="n">
-        <v>0.9259215720500775</v>
+        <v>0.7853978284292704</v>
       </c>
       <c r="D122" t="n">
-        <v>15.27913347597019</v>
+        <v>15.53397222900509</v>
       </c>
       <c r="E122" t="n">
         <v>-0.023293</v>
       </c>
       <c r="F122" t="n">
-        <v>0.01689971264367816</v>
+        <v>0.00336385542168675</v>
       </c>
       <c r="G122" t="n">
         <v>2.850097157933767</v>
@@ -3197,19 +3197,19 @@
         <v>42430</v>
       </c>
       <c r="B123" t="n">
-        <v>-0.02264002325581395</v>
+        <v>0.1814087471264368</v>
       </c>
       <c r="C123" t="n">
-        <v>0.7597218312828372</v>
+        <v>7.392684711559196</v>
       </c>
       <c r="D123" t="n">
-        <v>14.93321353874554</v>
+        <v>18.35197066896577</v>
       </c>
       <c r="E123" t="n">
         <v>0.118375</v>
       </c>
       <c r="F123" t="n">
-        <v>-0.1410150232558139</v>
+        <v>0.06303374712643679</v>
       </c>
       <c r="G123" t="n">
         <v>3.187477409004176</v>
@@ -3220,19 +3220,19 @@
         <v>42461</v>
       </c>
       <c r="B124" t="n">
-        <v>0.0209636923076923</v>
+        <v>-0.002496873563218394</v>
       </c>
       <c r="C124" t="n">
-        <v>1.282695510970167</v>
+        <v>0.9704455807055528</v>
       </c>
       <c r="D124" t="n">
-        <v>15.24626883253687</v>
+        <v>18.30614811856947</v>
       </c>
       <c r="E124" t="n">
         <v>-0.019062</v>
       </c>
       <c r="F124" t="n">
-        <v>0.0400256923076923</v>
+        <v>0.0165651264367816</v>
       </c>
       <c r="G124" t="n">
         <v>3.126717714633739</v>
@@ -3243,19 +3243,19 @@
         <v>42491</v>
       </c>
       <c r="B125" t="n">
-        <v>0.02058362637362637</v>
+        <v>-0.02983936363636364</v>
       </c>
       <c r="C125" t="n">
-        <v>1.276977243456524</v>
+        <v>0.6952224585670095</v>
       </c>
       <c r="D125" t="n">
-        <v>15.56009233377767</v>
+        <v>17.75990430807834</v>
       </c>
       <c r="E125" t="n">
         <v>0.00406</v>
       </c>
       <c r="F125" t="n">
-        <v>0.01652362637362637</v>
+        <v>-0.03389936363636364</v>
       </c>
       <c r="G125" t="n">
         <v>3.139412188555152</v>
@@ -3266,19 +3266,19 @@
         <v>42522</v>
       </c>
       <c r="B126" t="n">
-        <v>0.0572255054945055</v>
+        <v>0.04691986206896552</v>
       </c>
       <c r="C126" t="n">
-        <v>1.949896604164191</v>
+        <v>1.733649390885564</v>
       </c>
       <c r="D126" t="n">
-        <v>16.45052648311928</v>
+        <v>18.5931965685714</v>
       </c>
       <c r="E126" t="n">
         <v>-0.004934</v>
       </c>
       <c r="F126" t="n">
-        <v>0.0621595054945055</v>
+        <v>0.05185386206896552</v>
       </c>
       <c r="G126" t="n">
         <v>3.12392232881682</v>
@@ -3289,19 +3289,19 @@
         <v>42552</v>
       </c>
       <c r="B127" t="n">
-        <v>0.003738741573033708</v>
+        <v>0.02480077380952381</v>
       </c>
       <c r="C127" t="n">
-        <v>1.045799054003348</v>
+        <v>1.341755351081248</v>
       </c>
       <c r="D127" t="n">
-        <v>16.51203075038001</v>
+        <v>19.05432223106455</v>
       </c>
       <c r="E127" t="n">
         <v>0.015856</v>
       </c>
       <c r="F127" t="n">
-        <v>-0.01211725842696629</v>
+        <v>0.008944773809523809</v>
       </c>
       <c r="G127" t="n">
         <v>3.17345524126254</v>
@@ -3312,19 +3312,19 @@
         <v>42583</v>
       </c>
       <c r="B128" t="n">
-        <v>0.03003229545454545</v>
+        <v>0.04204848837209302</v>
       </c>
       <c r="C128" t="n">
-        <v>1.426297432912673</v>
+        <v>1.639287529708633</v>
       </c>
       <c r="D128" t="n">
-        <v>17.00792493642997</v>
+        <v>19.85552767783559</v>
       </c>
       <c r="E128" t="n">
         <v>0.03866</v>
       </c>
       <c r="F128" t="n">
-        <v>-0.008627704545454546</v>
+        <v>0.003388488372093025</v>
       </c>
       <c r="G128" t="n">
         <v>3.29614102088975</v>
@@ -3335,19 +3335,19 @@
         <v>42614</v>
       </c>
       <c r="B129" t="n">
-        <v>0.04250450574712644</v>
+        <v>-0.01588668604651163</v>
       </c>
       <c r="C129" t="n">
-        <v>1.647916826559349</v>
+        <v>0.8251659302979832</v>
       </c>
       <c r="D129" t="n">
-        <v>17.73083837963715</v>
+        <v>19.54008914332999</v>
       </c>
       <c r="E129" t="n">
         <v>-0.02239</v>
       </c>
       <c r="F129" t="n">
-        <v>0.06489450574712644</v>
+        <v>0.006503313953488368</v>
       </c>
       <c r="G129" t="n">
         <v>3.222340423432029</v>
@@ -3358,19 +3358,19 @@
         <v>42644</v>
       </c>
       <c r="B130" t="n">
-        <v>-0.03171676136363637</v>
+        <v>0.03982311764705883</v>
       </c>
       <c r="C130" t="n">
-        <v>0.6792489399488505</v>
+        <v>1.597767646421152</v>
       </c>
       <c r="D130" t="n">
-        <v>17.16847360997299</v>
+        <v>20.31823641211884</v>
       </c>
       <c r="E130" t="n">
         <v>0.025511</v>
       </c>
       <c r="F130" t="n">
-        <v>-0.05722776136363637</v>
+        <v>0.01431211764705883</v>
       </c>
       <c r="G130" t="n">
         <v>3.304545549974203</v>
@@ -3381,19 +3381,19 @@
         <v>42675</v>
       </c>
       <c r="B131" t="n">
-        <v>-0.01461673033707865</v>
+        <v>0.04920224418604652</v>
       </c>
       <c r="C131" t="n">
-        <v>0.8380351059583455</v>
+        <v>1.779551374066753</v>
       </c>
       <c r="D131" t="n">
-        <v>16.91752666091676</v>
+        <v>21.31793924149773</v>
       </c>
       <c r="E131" t="n">
         <v>0.060463</v>
       </c>
       <c r="F131" t="n">
-        <v>-0.07507973033707865</v>
+        <v>-0.01126075581395349</v>
       </c>
       <c r="G131" t="n">
         <v>3.504348287562293</v>
@@ -3404,19 +3404,19 @@
         <v>42705</v>
       </c>
       <c r="B132" t="n">
-        <v>0.0385456590909091</v>
+        <v>-0.009869267441860464</v>
       </c>
       <c r="C132" t="n">
-        <v>1.574371204039567</v>
+        <v>0.8877904906383737</v>
       </c>
       <c r="D132" t="n">
-        <v>17.56962387624982</v>
+        <v>21.10754679781406</v>
       </c>
       <c r="E132" t="n">
         <v>-0.06442100000000001</v>
       </c>
       <c r="F132" t="n">
-        <v>0.1029666590909091</v>
+        <v>0.05455173255813954</v>
       </c>
       <c r="G132" t="n">
         <v>3.278594666529242</v>
@@ -3427,19 +3427,19 @@
         <v>42736</v>
       </c>
       <c r="B133" t="n">
-        <v>-0.01771414606741573</v>
+        <v>-0.02350960975609756</v>
       </c>
       <c r="C133" t="n">
-        <v>0.8069649594313111</v>
+        <v>0.7516500391621264</v>
       </c>
       <c r="D133" t="n">
-        <v>17.25839299255638</v>
+        <v>20.61131660968888</v>
       </c>
       <c r="E133" t="n">
         <v>0.023528</v>
       </c>
       <c r="F133" t="n">
-        <v>-0.04124214606741573</v>
+        <v>-0.04703760975609756</v>
       </c>
       <c r="G133" t="n">
         <v>3.355733441843343</v>
@@ -3450,19 +3450,19 @@
         <v>42767</v>
       </c>
       <c r="B134" t="n">
-        <v>-0.03901911111111111</v>
+        <v>0.03477873809523809</v>
       </c>
       <c r="C134" t="n">
-        <v>0.6202646216915023</v>
+        <v>1.507196783790948</v>
       </c>
       <c r="D134" t="n">
-        <v>16.5849858387806</v>
+        <v>21.32815219185528</v>
       </c>
       <c r="E134" t="n">
         <v>0.019141</v>
       </c>
       <c r="F134" t="n">
-        <v>-0.05816011111111111</v>
+        <v>0.01563773809523809</v>
       </c>
       <c r="G134" t="n">
         <v>3.419965535653666</v>
@@ -3473,19 +3473,19 @@
         <v>42795</v>
       </c>
       <c r="B135" t="n">
-        <v>-0.06921449438202247</v>
+        <v>-0.01089603488372093</v>
       </c>
       <c r="C135" t="n">
-        <v>0.4228587687777309</v>
+        <v>0.8768055989153415</v>
       </c>
       <c r="D135" t="n">
-        <v>15.4370644296164</v>
+        <v>21.09575990156752</v>
       </c>
       <c r="E135" t="n">
         <v>0.0009369999999999999</v>
       </c>
       <c r="F135" t="n">
-        <v>-0.07015149438202246</v>
+        <v>-0.01183303488372093</v>
       </c>
       <c r="G135" t="n">
         <v>3.423170043360574</v>
@@ -3496,19 +3496,19 @@
         <v>42826</v>
       </c>
       <c r="B136" t="n">
-        <v>0.04280208139534884</v>
+        <v>-0.05748129411764707</v>
       </c>
       <c r="C136" t="n">
-        <v>1.653570333247218</v>
+        <v>0.4914504525110471</v>
       </c>
       <c r="D136" t="n">
-        <v>16.09780291783808</v>
+        <v>19.88314832203025</v>
       </c>
       <c r="E136" t="n">
         <v>-0.004714</v>
       </c>
       <c r="F136" t="n">
-        <v>0.04751608139534885</v>
+        <v>-0.05276729411764707</v>
       </c>
       <c r="G136" t="n">
         <v>3.407033219776172</v>
@@ -3519,19 +3519,19 @@
         <v>42856</v>
       </c>
       <c r="B137" t="n">
-        <v>0.009967482758620692</v>
+        <v>-0.07546861904761905</v>
       </c>
       <c r="C137" t="n">
-        <v>1.12638976572826</v>
+        <v>0.3899957566314116</v>
       </c>
       <c r="D137" t="n">
-        <v>16.25825749087331</v>
+        <v>18.38259457584764</v>
       </c>
       <c r="E137" t="n">
         <v>0.015446</v>
       </c>
       <c r="F137" t="n">
-        <v>-0.005478517241379309</v>
+        <v>-0.09091461904761905</v>
       </c>
       <c r="G137" t="n">
         <v>3.459658254888835</v>
@@ -3542,19 +3542,19 @@
         <v>42887</v>
       </c>
       <c r="B138" t="n">
-        <v>0.02193356818181818</v>
+        <v>0.03646303571428571</v>
       </c>
       <c r="C138" t="n">
-        <v>1.297394282215545</v>
+        <v>1.536900730416051</v>
       </c>
       <c r="D138" t="n">
-        <v>16.61485909006694</v>
+        <v>19.05287977838801</v>
       </c>
       <c r="E138" t="n">
         <v>0.049791</v>
       </c>
       <c r="F138" t="n">
-        <v>-0.02785743181818182</v>
+        <v>-0.01332796428571429</v>
       </c>
       <c r="G138" t="n">
         <v>3.631918099058004</v>
@@ -3565,19 +3565,19 @@
         <v>42917</v>
       </c>
       <c r="B139" t="n">
-        <v>0.0141179</v>
+        <v>-0.007379761904761902</v>
       </c>
       <c r="C139" t="n">
-        <v>1.183208773196185</v>
+        <v>0.9149503067392083</v>
       </c>
       <c r="D139" t="n">
-        <v>16.84942600921459</v>
+        <v>18.91227406202346</v>
       </c>
       <c r="E139" t="n">
         <v>0.019383</v>
       </c>
       <c r="F139" t="n">
-        <v>-0.0052651</v>
+        <v>-0.0267627619047619</v>
       </c>
       <c r="G139" t="n">
         <v>3.702315567572045</v>
@@ -3588,19 +3588,19 @@
         <v>42948</v>
       </c>
       <c r="B140" t="n">
-        <v>-0.0202444945054945</v>
+        <v>0.02191935294117647</v>
       </c>
       <c r="C140" t="n">
-        <v>0.7823706516808869</v>
+        <v>1.29717773552496</v>
       </c>
       <c r="D140" t="n">
-        <v>16.50831789695031</v>
+        <v>19.32681887210921</v>
       </c>
       <c r="E140" t="n">
         <v>0.022532</v>
       </c>
       <c r="F140" t="n">
-        <v>-0.04277649450549451</v>
+        <v>-0.0006126470588235303</v>
       </c>
       <c r="G140" t="n">
         <v>3.785736141940579</v>
@@ -3611,19 +3611,19 @@
         <v>42979</v>
       </c>
       <c r="B141" t="n">
-        <v>-0.05279534782608695</v>
+        <v>0.01262027586206897</v>
       </c>
       <c r="C141" t="n">
-        <v>0.5215859315999041</v>
+        <v>1.16241024514382</v>
       </c>
       <c r="D141" t="n">
-        <v>15.6367555115572</v>
+        <v>19.57072865781147</v>
       </c>
       <c r="E141" t="n">
         <v>0.00377</v>
       </c>
       <c r="F141" t="n">
-        <v>-0.05656534782608695</v>
+        <v>0.008850275862068966</v>
       </c>
       <c r="G141" t="n">
         <v>3.800008367195695</v>
@@ -3634,19 +3634,19 @@
         <v>43009</v>
       </c>
       <c r="B142" t="n">
-        <v>-0.007696866666666665</v>
+        <v>-0.006135470588235293</v>
       </c>
       <c r="C142" t="n">
-        <v>0.9114489572714362</v>
+        <v>0.9288087395074486</v>
       </c>
       <c r="D142" t="n">
-        <v>15.51640148928548</v>
+        <v>19.45065302774113</v>
       </c>
       <c r="E142" t="n">
         <v>0.044368</v>
       </c>
       <c r="F142" t="n">
-        <v>-0.05206486666666666</v>
+        <v>-0.05050347058823529</v>
       </c>
       <c r="G142" t="n">
         <v>3.968607138431433</v>
@@ -3657,19 +3657,19 @@
         <v>43040</v>
       </c>
       <c r="B143" t="n">
-        <v>0.1399125641025641</v>
+        <v>-0.06650650000000001</v>
       </c>
       <c r="C143" t="n">
-        <v>4.813472396946767</v>
+        <v>0.4378603089541067</v>
       </c>
       <c r="D143" t="n">
-        <v>17.68734100729626</v>
+        <v>18.15705817215167</v>
       </c>
       <c r="E143" t="n">
         <v>-0.000154</v>
       </c>
       <c r="F143" t="n">
-        <v>0.1400665641025641</v>
+        <v>-0.06635250000000001</v>
       </c>
       <c r="G143" t="n">
         <v>3.967995972932115</v>
@@ -3680,19 +3680,19 @@
         <v>43070</v>
       </c>
       <c r="B144" t="n">
-        <v>0.08485546835443038</v>
+        <v>-0.01914344318181818</v>
       </c>
       <c r="C144" t="n">
-        <v>2.657434625025588</v>
+        <v>0.7929868675458061</v>
       </c>
       <c r="D144" t="n">
-        <v>19.18820861241491</v>
+        <v>17.80946956068411</v>
       </c>
       <c r="E144" t="n">
         <v>0.00618</v>
       </c>
       <c r="F144" t="n">
-        <v>0.07867546835443037</v>
+        <v>-0.02532344318181818</v>
       </c>
       <c r="G144" t="n">
         <v>3.992518188044836</v>
@@ -3703,19 +3703,19 @@
         <v>43101</v>
       </c>
       <c r="B145" t="n">
-        <v>-0.0134634</v>
+        <v>-0.03420600000000001</v>
       </c>
       <c r="C145" t="n">
-        <v>0.8498815941911352</v>
+        <v>0.6585883380753182</v>
       </c>
       <c r="D145" t="n">
-        <v>18.92987008458252</v>
+        <v>17.20027884489135</v>
       </c>
       <c r="E145" t="n">
         <v>0.060792</v>
       </c>
       <c r="F145" t="n">
-        <v>-0.0742554</v>
+        <v>-0.094998</v>
       </c>
       <c r="G145" t="n">
         <v>4.235231353732457</v>
@@ -3726,19 +3726,19 @@
         <v>43132</v>
       </c>
       <c r="B146" t="n">
-        <v>-0.06641702197802196</v>
+        <v>-0.04957013953488372</v>
       </c>
       <c r="C146" t="n">
-        <v>0.4383642165102465</v>
+        <v>0.5433014566389885</v>
       </c>
       <c r="D146" t="n">
-        <v>17.6726044871337</v>
+        <v>16.34765862251118</v>
       </c>
       <c r="E146" t="n">
         <v>-0.05899500000000001</v>
       </c>
       <c r="F146" t="n">
-        <v>-0.007422021978021956</v>
+        <v>0.009424860465116286</v>
       </c>
       <c r="G146" t="n">
         <v>3.985373880019011</v>
@@ -3749,19 +3749,19 @@
         <v>43160</v>
       </c>
       <c r="B147" t="n">
-        <v>0.0193085054945055</v>
+        <v>0.03730436781609196</v>
       </c>
       <c r="C147" t="n">
-        <v>1.257962739813262</v>
+        <v>1.551938400262088</v>
       </c>
       <c r="D147" t="n">
-        <v>18.01383606797575</v>
+        <v>16.95749769269725</v>
       </c>
       <c r="E147" t="n">
         <v>-0.031102</v>
       </c>
       <c r="F147" t="n">
-        <v>0.0504105054945055</v>
+        <v>0.06840636781609195</v>
       </c>
       <c r="G147" t="n">
         <v>3.86142078160266</v>
@@ -3772,19 +3772,19 @@
         <v>43191</v>
       </c>
       <c r="B148" t="n">
-        <v>-0.04356784444444444</v>
+        <v>-0.0402935393258427</v>
       </c>
       <c r="C148" t="n">
-        <v>0.5859357892027924</v>
+        <v>0.6104653542098595</v>
       </c>
       <c r="D148" t="n">
-        <v>17.22901206031846</v>
+        <v>16.27422009254866</v>
       </c>
       <c r="E148" t="n">
         <v>-0.036327</v>
       </c>
       <c r="F148" t="n">
-        <v>-0.007240844444444443</v>
+        <v>-0.003966539325842698</v>
       </c>
       <c r="G148" t="n">
         <v>3.72114694886938</v>
@@ -3795,19 +3795,19 @@
         <v>43221</v>
       </c>
       <c r="B149" t="n">
-        <v>-0.004115945054945053</v>
+        <v>-0.01004656818181818</v>
       </c>
       <c r="C149" t="n">
-        <v>0.9517115665043948</v>
+        <v>0.8858846698422496</v>
       </c>
       <c r="D149" t="n">
-        <v>17.1580983933272</v>
+        <v>16.11072003078296</v>
       </c>
       <c r="E149" t="n">
         <v>0.012111</v>
       </c>
       <c r="F149" t="n">
-        <v>-0.01622694505494506</v>
+        <v>-0.02215756818181818</v>
       </c>
       <c r="G149" t="n">
         <v>3.766213759567137</v>
@@ -3818,19 +3818,19 @@
         <v>43252</v>
       </c>
       <c r="B150" t="n">
-        <v>-0.1130563626373626</v>
+        <v>-0.1146657</v>
       </c>
       <c r="C150" t="n">
-        <v>0.237002141920458</v>
+        <v>0.2318929161373983</v>
       </c>
       <c r="D150" t="n">
-        <v>15.21826619920365</v>
+        <v>14.26337304094921</v>
       </c>
       <c r="E150" t="n">
         <v>-0.07663400000000001</v>
       </c>
       <c r="F150" t="n">
-        <v>-0.03642236263736262</v>
+        <v>-0.03803170000000003</v>
       </c>
       <c r="G150" t="n">
         <v>3.477593734316469</v>
@@ -3841,19 +3841,19 @@
         <v>43282</v>
       </c>
       <c r="B151" t="n">
-        <v>-0.007199771739130438</v>
+        <v>0.02912328089887641</v>
       </c>
       <c r="C151" t="n">
-        <v>0.9169431703372847</v>
+        <v>1.411265859360274</v>
       </c>
       <c r="D151" t="n">
-        <v>15.10869815630406</v>
+        <v>14.67876926058623</v>
       </c>
       <c r="E151" t="n">
         <v>0.0019</v>
       </c>
       <c r="F151" t="n">
-        <v>-0.009099771739130439</v>
+        <v>0.02722328089887641</v>
       </c>
       <c r="G151" t="n">
         <v>3.48420116241167</v>
@@ -3864,19 +3864,19 @@
         <v>43313</v>
       </c>
       <c r="B152" t="n">
-        <v>-0.07951581720430109</v>
+        <v>-0.0677105888888889</v>
       </c>
       <c r="C152" t="n">
-        <v>0.369995091082942</v>
+        <v>0.4311307689409581</v>
       </c>
       <c r="D152" t="n">
-        <v>13.90731767551243</v>
+        <v>13.68486114978782</v>
       </c>
       <c r="E152" t="n">
         <v>-0.052067</v>
       </c>
       <c r="F152" t="n">
-        <v>-0.0274488172043011</v>
+        <v>-0.0156435888888889</v>
       </c>
       <c r="G152" t="n">
         <v>3.302789260488382</v>
@@ -3887,19 +3887,19 @@
         <v>43344</v>
       </c>
       <c r="B153" t="n">
-        <v>0.005524510638297874</v>
+        <v>-0.006065764044943818</v>
       </c>
       <c r="C153" t="n">
-        <v>1.068346021259272</v>
+        <v>0.9295907659393564</v>
       </c>
       <c r="D153" t="n">
-        <v>13.98414879996099</v>
+        <v>13.60185201106539</v>
       </c>
       <c r="E153" t="n">
         <v>0.03129700000000001</v>
       </c>
       <c r="F153" t="n">
-        <v>-0.02577248936170213</v>
+        <v>-0.03736276404494383</v>
       </c>
       <c r="G153" t="n">
         <v>3.406156655973887</v>
@@ -3910,19 +3910,19 @@
         <v>43374</v>
       </c>
       <c r="B154" t="n">
-        <v>-0.0900061914893617</v>
+        <v>-0.09374778888888889</v>
       </c>
       <c r="C154" t="n">
-        <v>0.3224491595608177</v>
+        <v>0.3068943904479383</v>
       </c>
       <c r="D154" t="n">
-        <v>12.72548882525597</v>
+        <v>12.32670846023412</v>
       </c>
       <c r="E154" t="n">
         <v>-0.082888</v>
       </c>
       <c r="F154" t="n">
-        <v>-0.0071181914893617</v>
+        <v>-0.01085978888888889</v>
       </c>
       <c r="G154" t="n">
         <v>3.123827143073524</v>
@@ -3933,19 +3933,19 @@
         <v>43405</v>
       </c>
       <c r="B155" t="n">
-        <v>0.06951641489361701</v>
+        <v>0.05514883516483517</v>
       </c>
       <c r="C155" t="n">
-        <v>2.24000740440626</v>
+        <v>1.904428560924255</v>
       </c>
       <c r="D155" t="n">
-        <v>13.61011918615655</v>
+        <v>13.00651207323255</v>
       </c>
       <c r="E155" t="n">
         <v>0.005982</v>
       </c>
       <c r="F155" t="n">
-        <v>0.06353441489361701</v>
+        <v>0.04916683516483517</v>
       </c>
       <c r="G155" t="n">
         <v>3.142513877043389</v>
@@ -3956,19 +3956,19 @@
         <v>43435</v>
       </c>
       <c r="B156" t="n">
-        <v>-0.04430612765957447</v>
+        <v>-0.02976175824175825</v>
       </c>
       <c r="C156" t="n">
-        <v>0.5805312693028537</v>
+        <v>0.6958901016923404</v>
       </c>
       <c r="D156" t="n">
-        <v>13.00710750803267</v>
+        <v>12.6194154053405</v>
       </c>
       <c r="E156" t="n">
         <v>-0.051072</v>
       </c>
       <c r="F156" t="n">
-        <v>0.006765872340425527</v>
+        <v>0.02131024175824175</v>
       </c>
       <c r="G156" t="n">
         <v>2.982019408315029</v>
@@ -3979,19 +3979,19 @@
         <v>43466</v>
       </c>
       <c r="B157" t="n">
-        <v>0.001653627659574469</v>
+        <v>-0.0002287142857142829</v>
       </c>
       <c r="C157" t="n">
-        <v>1.020025006399032</v>
+        <v>0.9972588784154983</v>
       </c>
       <c r="D157" t="n">
-        <v>13.02861642077901</v>
+        <v>12.61652916475993</v>
       </c>
       <c r="E157" t="n">
         <v>0.063434</v>
       </c>
       <c r="F157" t="n">
-        <v>-0.06178037234042554</v>
+        <v>-0.06366271428571428</v>
       </c>
       <c r="G157" t="n">
         <v>3.171180827462085</v>
@@ -4002,19 +4002,19 @@
         <v>43497</v>
       </c>
       <c r="B158" t="n">
-        <v>0.2170311808510638</v>
+        <v>0.2051381208791208</v>
       </c>
       <c r="C158" t="n">
-        <v>10.55894340633214</v>
+        <v>9.385164540037454</v>
       </c>
       <c r="D158" t="n">
-        <v>15.85623242743624</v>
+        <v>15.20466024963541</v>
       </c>
       <c r="E158" t="n">
         <v>0.146093</v>
       </c>
       <c r="F158" t="n">
-        <v>0.07093818085106382</v>
+        <v>0.05904512087912084</v>
       </c>
       <c r="G158" t="n">
         <v>3.634468148088503</v>

</xml_diff>